<commit_message>
reworking enums in db
</commit_message>
<xml_diff>
--- a/doc/Metadata ALM tools.xlsx
+++ b/doc/Metadata ALM tools.xlsx
@@ -49069,9 +49069,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
pumpy na GitHub a Redmine, GUI, major refactoring
</commit_message>
<xml_diff>
--- a/doc/Metadata ALM tools.xlsx
+++ b/doc/Metadata ALM tools.xlsx
@@ -6618,27 +6618,54 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -6648,33 +6675,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -34766,11 +34766,11 @@
       <c r="G123" s="224" t="s">
         <v>131</v>
       </c>
-      <c r="H123" s="222"/>
-      <c r="I123" s="225" t="s">
+      <c r="H123" s="223"/>
+      <c r="I123" s="228" t="s">
         <v>132</v>
       </c>
-      <c r="J123" s="222"/>
+      <c r="J123" s="223"/>
       <c r="K123" s="63"/>
       <c r="L123" s="57"/>
       <c r="M123" s="75"/>
@@ -35329,10 +35329,10 @@
       <c r="AG132" s="34"/>
     </row>
     <row r="133" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A133" s="226" t="s">
+      <c r="A133" s="221" t="s">
         <v>901</v>
       </c>
-      <c r="B133" s="226"/>
+      <c r="B133" s="221"/>
       <c r="C133" s="83"/>
       <c r="D133" s="51">
         <f t="shared" si="6"/>
@@ -35372,8 +35372,8 @@
       <c r="AG133" s="34"/>
     </row>
     <row r="134" spans="1:33" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A134" s="226"/>
-      <c r="B134" s="226"/>
+      <c r="A134" s="221"/>
+      <c r="B134" s="221"/>
       <c r="C134" s="83"/>
       <c r="D134" s="51">
         <f t="shared" si="6"/>
@@ -36467,8 +36467,8 @@
       <c r="H155" s="53" t="s">
         <v>598</v>
       </c>
-      <c r="I155" s="227"/>
-      <c r="J155" s="222"/>
+      <c r="I155" s="222"/>
+      <c r="J155" s="223"/>
       <c r="K155" s="56" t="s">
         <v>20</v>
       </c>
@@ -37294,7 +37294,7 @@
       <c r="G171" s="224" t="s">
         <v>163</v>
       </c>
-      <c r="H171" s="222"/>
+      <c r="H171" s="223"/>
       <c r="I171" s="124"/>
       <c r="J171" s="125"/>
       <c r="K171" s="63"/>
@@ -37836,22 +37836,22 @@
       <c r="F182" s="145"/>
       <c r="G182" s="87"/>
       <c r="H182" s="73"/>
-      <c r="I182" s="227" t="s">
+      <c r="I182" s="222" t="s">
         <v>726</v>
       </c>
-      <c r="J182" s="222"/>
-      <c r="K182" s="228" t="s">
+      <c r="J182" s="223"/>
+      <c r="K182" s="225" t="s">
         <v>168</v>
       </c>
-      <c r="L182" s="222"/>
-      <c r="M182" s="221" t="s">
+      <c r="L182" s="223"/>
+      <c r="M182" s="226" t="s">
         <v>746</v>
       </c>
-      <c r="N182" s="222"/>
-      <c r="O182" s="223" t="s">
+      <c r="N182" s="223"/>
+      <c r="O182" s="227" t="s">
         <v>169</v>
       </c>
-      <c r="P182" s="222"/>
+      <c r="P182" s="223"/>
       <c r="Q182" s="29"/>
       <c r="R182" s="29"/>
       <c r="W182" s="34"/>
@@ -38147,7 +38147,7 @@
       <c r="G188" s="224" t="s">
         <v>175</v>
       </c>
-      <c r="H188" s="222"/>
+      <c r="H188" s="223"/>
       <c r="I188" s="77"/>
       <c r="J188" s="71"/>
       <c r="K188" s="63"/>
@@ -39616,7 +39616,7 @@
       <c r="G217" s="224" t="s">
         <v>184</v>
       </c>
-      <c r="H217" s="222"/>
+      <c r="H217" s="223"/>
       <c r="I217" s="77"/>
       <c r="J217" s="71"/>
       <c r="K217" s="56"/>
@@ -42573,17 +42573,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A133:B134"/>
-    <mergeCell ref="I155:J155"/>
-    <mergeCell ref="G171:H171"/>
-    <mergeCell ref="I182:J182"/>
-    <mergeCell ref="K182:L182"/>
     <mergeCell ref="M182:N182"/>
     <mergeCell ref="O182:P182"/>
     <mergeCell ref="G188:H188"/>
     <mergeCell ref="G217:H217"/>
     <mergeCell ref="G123:H123"/>
     <mergeCell ref="I123:J123"/>
+    <mergeCell ref="A133:B134"/>
+    <mergeCell ref="I155:J155"/>
+    <mergeCell ref="G171:H171"/>
+    <mergeCell ref="I182:J182"/>
+    <mergeCell ref="K182:L182"/>
   </mergeCells>
   <conditionalFormatting sqref="F2">
     <cfRule type="colorScale" priority="2">
@@ -42672,43 +42672,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="232" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239" t="s">
+      <c r="B1" s="232"/>
+      <c r="C1" s="232"/>
+      <c r="D1" s="232" t="s">
         <v>259</v>
       </c>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239" t="s">
+      <c r="E1" s="232"/>
+      <c r="F1" s="232" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="239"/>
-      <c r="H1" s="239" t="s">
+      <c r="G1" s="232"/>
+      <c r="H1" s="232" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="239"/>
-      <c r="J1" s="239" t="s">
+      <c r="I1" s="232"/>
+      <c r="J1" s="232" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="239"/>
-      <c r="L1" s="239" t="s">
+      <c r="K1" s="232"/>
+      <c r="L1" s="232" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="239"/>
-      <c r="N1" s="239" t="s">
+      <c r="M1" s="232"/>
+      <c r="N1" s="232" t="s">
         <v>261</v>
       </c>
-      <c r="O1" s="239"/>
-      <c r="P1" s="239" t="s">
+      <c r="O1" s="232"/>
+      <c r="P1" s="232" t="s">
         <v>263</v>
       </c>
-      <c r="Q1" s="239"/>
-      <c r="R1" s="239" t="s">
+      <c r="Q1" s="232"/>
+      <c r="R1" s="232" t="s">
         <v>262</v>
       </c>
-      <c r="S1" s="239"/>
+      <c r="S1" s="232"/>
     </row>
     <row r="2" spans="1:19" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
@@ -42791,7 +42791,7 @@
       <c r="S3" s="15"/>
     </row>
     <row r="4" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="236" t="s">
+      <c r="A4" s="229" t="s">
         <v>265</v>
       </c>
       <c r="B4" s="24" t="s">
@@ -42800,108 +42800,108 @@
       <c r="C4" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="D4" s="235" t="s">
+      <c r="D4" s="233" t="s">
         <v>1400</v>
       </c>
-      <c r="E4" s="235"/>
-      <c r="F4" s="235"/>
-      <c r="G4" s="235"/>
-      <c r="H4" s="235"/>
-      <c r="I4" s="235"/>
-      <c r="J4" s="235"/>
-      <c r="K4" s="235"/>
-      <c r="L4" s="235"/>
-      <c r="M4" s="235"/>
-      <c r="N4" s="235"/>
-      <c r="O4" s="235"/>
+      <c r="E4" s="233"/>
+      <c r="F4" s="233"/>
+      <c r="G4" s="233"/>
+      <c r="H4" s="233"/>
+      <c r="I4" s="233"/>
+      <c r="J4" s="233"/>
+      <c r="K4" s="233"/>
+      <c r="L4" s="233"/>
+      <c r="M4" s="233"/>
+      <c r="N4" s="233"/>
+      <c r="O4" s="233"/>
     </row>
     <row r="5" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="236"/>
+      <c r="A5" s="229"/>
       <c r="B5" s="24" t="s">
         <v>98</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="D5" s="235"/>
-      <c r="E5" s="235"/>
-      <c r="F5" s="235"/>
-      <c r="G5" s="235"/>
-      <c r="H5" s="235"/>
-      <c r="I5" s="235"/>
-      <c r="J5" s="235"/>
-      <c r="K5" s="235"/>
-      <c r="L5" s="235"/>
-      <c r="M5" s="235"/>
-      <c r="N5" s="235"/>
-      <c r="O5" s="235"/>
+      <c r="D5" s="233"/>
+      <c r="E5" s="233"/>
+      <c r="F5" s="233"/>
+      <c r="G5" s="233"/>
+      <c r="H5" s="233"/>
+      <c r="I5" s="233"/>
+      <c r="J5" s="233"/>
+      <c r="K5" s="233"/>
+      <c r="L5" s="233"/>
+      <c r="M5" s="233"/>
+      <c r="N5" s="233"/>
+      <c r="O5" s="233"/>
     </row>
     <row r="6" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="236"/>
+      <c r="A6" s="229"/>
       <c r="B6" s="24" t="s">
         <v>267</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="D6" s="235"/>
-      <c r="E6" s="235"/>
-      <c r="F6" s="235"/>
-      <c r="G6" s="235"/>
-      <c r="H6" s="235"/>
-      <c r="I6" s="235"/>
-      <c r="J6" s="235"/>
-      <c r="K6" s="235"/>
-      <c r="L6" s="235"/>
-      <c r="M6" s="235"/>
-      <c r="N6" s="235"/>
-      <c r="O6" s="235"/>
+      <c r="D6" s="233"/>
+      <c r="E6" s="233"/>
+      <c r="F6" s="233"/>
+      <c r="G6" s="233"/>
+      <c r="H6" s="233"/>
+      <c r="I6" s="233"/>
+      <c r="J6" s="233"/>
+      <c r="K6" s="233"/>
+      <c r="L6" s="233"/>
+      <c r="M6" s="233"/>
+      <c r="N6" s="233"/>
+      <c r="O6" s="233"/>
     </row>
     <row r="7" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="236"/>
+      <c r="A7" s="229"/>
       <c r="B7" s="24" t="s">
         <v>137</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="D7" s="235"/>
-      <c r="E7" s="235"/>
-      <c r="F7" s="235"/>
-      <c r="G7" s="235"/>
-      <c r="H7" s="235"/>
-      <c r="I7" s="235"/>
-      <c r="J7" s="235"/>
-      <c r="K7" s="235"/>
-      <c r="L7" s="235"/>
-      <c r="M7" s="235"/>
-      <c r="N7" s="235"/>
-      <c r="O7" s="235"/>
+      <c r="D7" s="233"/>
+      <c r="E7" s="233"/>
+      <c r="F7" s="233"/>
+      <c r="G7" s="233"/>
+      <c r="H7" s="233"/>
+      <c r="I7" s="233"/>
+      <c r="J7" s="233"/>
+      <c r="K7" s="233"/>
+      <c r="L7" s="233"/>
+      <c r="M7" s="233"/>
+      <c r="N7" s="233"/>
+      <c r="O7" s="233"/>
     </row>
     <row r="8" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="236"/>
+      <c r="A8" s="229"/>
       <c r="B8" s="24" t="s">
         <v>136</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="D8" s="235"/>
-      <c r="E8" s="235"/>
-      <c r="F8" s="235"/>
-      <c r="G8" s="235"/>
-      <c r="H8" s="235"/>
-      <c r="I8" s="235"/>
-      <c r="J8" s="235"/>
-      <c r="K8" s="235"/>
-      <c r="L8" s="235"/>
-      <c r="M8" s="235"/>
-      <c r="N8" s="235"/>
-      <c r="O8" s="235"/>
+      <c r="D8" s="233"/>
+      <c r="E8" s="233"/>
+      <c r="F8" s="233"/>
+      <c r="G8" s="233"/>
+      <c r="H8" s="233"/>
+      <c r="I8" s="233"/>
+      <c r="J8" s="233"/>
+      <c r="K8" s="233"/>
+      <c r="L8" s="233"/>
+      <c r="M8" s="233"/>
+      <c r="N8" s="233"/>
+      <c r="O8" s="233"/>
     </row>
     <row r="9" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" s="237" t="s">
+      <c r="A10" s="231" t="s">
         <v>269</v>
       </c>
       <c r="B10" t="s">
@@ -42954,7 +42954,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="232"/>
+      <c r="A11" s="230"/>
       <c r="B11" t="s">
         <v>98</v>
       </c>
@@ -43011,7 +43011,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="232"/>
+      <c r="A12" s="230"/>
       <c r="B12" t="s">
         <v>267</v>
       </c>
@@ -43050,7 +43050,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="232"/>
+      <c r="A13" s="230"/>
       <c r="B13" t="s">
         <v>52</v>
       </c>
@@ -43089,7 +43089,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="232"/>
+      <c r="A14" s="230"/>
       <c r="B14" t="s">
         <v>31</v>
       </c>
@@ -43122,7 +43122,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="232"/>
+      <c r="A15" s="230"/>
       <c r="B15" t="s">
         <v>105</v>
       </c>
@@ -43163,7 +43163,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="232"/>
+      <c r="A16" s="230"/>
       <c r="B16" s="10" t="s">
         <v>433</v>
       </c>
@@ -43202,7 +43202,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="232"/>
+      <c r="A17" s="230"/>
       <c r="B17" s="10" t="s">
         <v>1426</v>
       </c>
@@ -43235,7 +43235,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="232"/>
+      <c r="A18" s="230"/>
       <c r="B18" t="s">
         <v>115</v>
       </c>
@@ -43265,7 +43265,7 @@
     </row>
     <row r="19" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A20" s="232" t="s">
+      <c r="A20" s="230" t="s">
         <v>270</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -43288,7 +43288,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A21" s="232"/>
+      <c r="A21" s="230"/>
       <c r="B21" s="6" t="s">
         <v>98</v>
       </c>
@@ -43317,7 +43317,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A22" s="232"/>
+      <c r="A22" s="230"/>
       <c r="B22" s="10" t="s">
         <v>435</v>
       </c>
@@ -43339,7 +43339,7 @@
     </row>
     <row r="23" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:19" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="237" t="s">
+      <c r="A24" s="231" t="s">
         <v>348</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -43382,7 +43382,7 @@
       <c r="S24" s="10"/>
     </row>
     <row r="25" spans="1:19" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="237"/>
+      <c r="A25" s="231"/>
       <c r="B25" s="10" t="s">
         <v>98</v>
       </c>
@@ -43427,7 +43427,7 @@
       <c r="S25" s="10"/>
     </row>
     <row r="26" spans="1:19" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="237"/>
+      <c r="A26" s="231"/>
       <c r="B26" s="10" t="s">
         <v>2</v>
       </c>
@@ -43468,7 +43468,7 @@
       <c r="S26" s="10"/>
     </row>
     <row r="27" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="237"/>
+      <c r="A27" s="231"/>
       <c r="B27" s="10" t="s">
         <v>281</v>
       </c>
@@ -43514,7 +43514,7 @@
     </row>
     <row r="28" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="236" t="s">
+      <c r="A29" s="229" t="s">
         <v>271</v>
       </c>
       <c r="B29" s="25" t="s">
@@ -43523,78 +43523,78 @@
       <c r="C29" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D29" s="236" t="s">
+      <c r="D29" s="229" t="s">
         <v>1403</v>
       </c>
-      <c r="E29" s="236"/>
-      <c r="F29" s="236"/>
-      <c r="G29" s="236"/>
-      <c r="H29" s="236"/>
-      <c r="I29" s="236"/>
-      <c r="J29" s="236"/>
-      <c r="K29" s="236"/>
-      <c r="L29" s="236"/>
-      <c r="M29" s="236"/>
-      <c r="N29" s="236"/>
-      <c r="O29" s="236"/>
-      <c r="P29" s="236"/>
-      <c r="Q29" s="236"/>
-      <c r="R29" s="236"/>
-      <c r="S29" s="236"/>
+      <c r="E29" s="229"/>
+      <c r="F29" s="229"/>
+      <c r="G29" s="229"/>
+      <c r="H29" s="229"/>
+      <c r="I29" s="229"/>
+      <c r="J29" s="229"/>
+      <c r="K29" s="229"/>
+      <c r="L29" s="229"/>
+      <c r="M29" s="229"/>
+      <c r="N29" s="229"/>
+      <c r="O29" s="229"/>
+      <c r="P29" s="229"/>
+      <c r="Q29" s="229"/>
+      <c r="R29" s="229"/>
+      <c r="S29" s="229"/>
     </row>
     <row r="30" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="236"/>
+      <c r="A30" s="229"/>
       <c r="B30" s="25" t="s">
         <v>98</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D30" s="236"/>
-      <c r="E30" s="236"/>
-      <c r="F30" s="236"/>
-      <c r="G30" s="236"/>
-      <c r="H30" s="236"/>
-      <c r="I30" s="236"/>
-      <c r="J30" s="236"/>
-      <c r="K30" s="236"/>
-      <c r="L30" s="236"/>
-      <c r="M30" s="236"/>
-      <c r="N30" s="236"/>
-      <c r="O30" s="236"/>
-      <c r="P30" s="236"/>
-      <c r="Q30" s="236"/>
-      <c r="R30" s="236"/>
-      <c r="S30" s="236"/>
+      <c r="D30" s="229"/>
+      <c r="E30" s="229"/>
+      <c r="F30" s="229"/>
+      <c r="G30" s="229"/>
+      <c r="H30" s="229"/>
+      <c r="I30" s="229"/>
+      <c r="J30" s="229"/>
+      <c r="K30" s="229"/>
+      <c r="L30" s="229"/>
+      <c r="M30" s="229"/>
+      <c r="N30" s="229"/>
+      <c r="O30" s="229"/>
+      <c r="P30" s="229"/>
+      <c r="Q30" s="229"/>
+      <c r="R30" s="229"/>
+      <c r="S30" s="229"/>
     </row>
     <row r="31" spans="1:19" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="236"/>
+      <c r="A31" s="229"/>
       <c r="B31" s="25" t="s">
         <v>267</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D31" s="236"/>
-      <c r="E31" s="236"/>
-      <c r="F31" s="236"/>
-      <c r="G31" s="236"/>
-      <c r="H31" s="236"/>
-      <c r="I31" s="236"/>
-      <c r="J31" s="236"/>
-      <c r="K31" s="236"/>
-      <c r="L31" s="236"/>
-      <c r="M31" s="236"/>
-      <c r="N31" s="236"/>
-      <c r="O31" s="236"/>
-      <c r="P31" s="236"/>
-      <c r="Q31" s="236"/>
-      <c r="R31" s="236"/>
-      <c r="S31" s="236"/>
+      <c r="D31" s="229"/>
+      <c r="E31" s="229"/>
+      <c r="F31" s="229"/>
+      <c r="G31" s="229"/>
+      <c r="H31" s="229"/>
+      <c r="I31" s="229"/>
+      <c r="J31" s="229"/>
+      <c r="K31" s="229"/>
+      <c r="L31" s="229"/>
+      <c r="M31" s="229"/>
+      <c r="N31" s="229"/>
+      <c r="O31" s="229"/>
+      <c r="P31" s="229"/>
+      <c r="Q31" s="229"/>
+      <c r="R31" s="229"/>
+      <c r="S31" s="229"/>
     </row>
     <row r="32" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="232" t="s">
+      <c r="A33" s="230" t="s">
         <v>272</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -43653,7 +43653,7 @@
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A34" s="232"/>
+      <c r="A34" s="230"/>
       <c r="B34" s="6" t="s">
         <v>98</v>
       </c>
@@ -43676,7 +43676,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" s="13" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="232"/>
+      <c r="A35" s="230"/>
       <c r="B35" s="10" t="s">
         <v>2</v>
       </c>
@@ -43733,7 +43733,7 @@
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="232"/>
+      <c r="A36" s="230"/>
       <c r="B36" s="6" t="s">
         <v>22</v>
       </c>
@@ -43750,7 +43750,7 @@
       </c>
     </row>
     <row r="37" spans="1:19" s="7" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="232"/>
+      <c r="A37" s="230"/>
       <c r="B37" s="10" t="s">
         <v>52</v>
       </c>
@@ -43807,7 +43807,7 @@
       </c>
     </row>
     <row r="38" spans="1:19" s="7" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="232"/>
+      <c r="A38" s="230"/>
       <c r="B38" s="10" t="s">
         <v>31</v>
       </c>
@@ -43864,7 +43864,7 @@
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A39" s="232"/>
+      <c r="A39" s="230"/>
       <c r="B39" s="10" t="s">
         <v>390</v>
       </c>
@@ -43921,7 +43921,7 @@
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A40" s="232"/>
+      <c r="A40" s="230"/>
       <c r="B40" s="6" t="s">
         <v>273</v>
       </c>
@@ -43951,59 +43951,59 @@
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A41" s="232"/>
+      <c r="A41" s="230"/>
       <c r="B41" s="6" t="s">
         <v>274</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>1428</v>
       </c>
-      <c r="D41" s="235" t="s">
+      <c r="D41" s="233" t="s">
         <v>1397</v>
       </c>
-      <c r="E41" s="235"/>
-      <c r="F41" s="235"/>
-      <c r="G41" s="235"/>
-      <c r="H41" s="235"/>
-      <c r="I41" s="235"/>
-      <c r="J41" s="235"/>
-      <c r="K41" s="235"/>
-      <c r="L41" s="235"/>
-      <c r="M41" s="235"/>
-      <c r="N41" s="235"/>
-      <c r="O41" s="235"/>
-      <c r="P41" s="235"/>
-      <c r="Q41" s="235"/>
-      <c r="R41" s="235"/>
-      <c r="S41" s="235"/>
+      <c r="E41" s="233"/>
+      <c r="F41" s="233"/>
+      <c r="G41" s="233"/>
+      <c r="H41" s="233"/>
+      <c r="I41" s="233"/>
+      <c r="J41" s="233"/>
+      <c r="K41" s="233"/>
+      <c r="L41" s="233"/>
+      <c r="M41" s="233"/>
+      <c r="N41" s="233"/>
+      <c r="O41" s="233"/>
+      <c r="P41" s="233"/>
+      <c r="Q41" s="233"/>
+      <c r="R41" s="233"/>
+      <c r="S41" s="233"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A42" s="232"/>
+      <c r="A42" s="230"/>
       <c r="B42" s="6" t="s">
         <v>268</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>1429</v>
       </c>
-      <c r="D42" s="235"/>
-      <c r="E42" s="235"/>
-      <c r="F42" s="235"/>
-      <c r="G42" s="235"/>
-      <c r="H42" s="235"/>
-      <c r="I42" s="235"/>
-      <c r="J42" s="235"/>
-      <c r="K42" s="235"/>
-      <c r="L42" s="235"/>
-      <c r="M42" s="235"/>
-      <c r="N42" s="235"/>
-      <c r="O42" s="235"/>
-      <c r="P42" s="235"/>
-      <c r="Q42" s="235"/>
-      <c r="R42" s="235"/>
-      <c r="S42" s="235"/>
+      <c r="D42" s="233"/>
+      <c r="E42" s="233"/>
+      <c r="F42" s="233"/>
+      <c r="G42" s="233"/>
+      <c r="H42" s="233"/>
+      <c r="I42" s="233"/>
+      <c r="J42" s="233"/>
+      <c r="K42" s="233"/>
+      <c r="L42" s="233"/>
+      <c r="M42" s="233"/>
+      <c r="N42" s="233"/>
+      <c r="O42" s="233"/>
+      <c r="P42" s="233"/>
+      <c r="Q42" s="233"/>
+      <c r="R42" s="233"/>
+      <c r="S42" s="233"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A43" s="232"/>
+      <c r="A43" s="230"/>
       <c r="B43" s="6" t="s">
         <v>275</v>
       </c>
@@ -44024,7 +44024,7 @@
       </c>
     </row>
     <row r="44" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="232"/>
+      <c r="A44" s="230"/>
       <c r="B44" s="6" t="s">
         <v>86</v>
       </c>
@@ -44052,7 +44052,7 @@
     </row>
     <row r="45" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="236" t="s">
+      <c r="A46" s="229" t="s">
         <v>276</v>
       </c>
       <c r="B46" s="24" t="s">
@@ -44061,78 +44061,78 @@
       <c r="C46" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="D46" s="235" t="s">
+      <c r="D46" s="233" t="s">
         <v>1403</v>
       </c>
-      <c r="E46" s="235"/>
-      <c r="F46" s="235"/>
-      <c r="G46" s="235"/>
-      <c r="H46" s="235"/>
-      <c r="I46" s="235"/>
-      <c r="J46" s="235"/>
-      <c r="K46" s="235"/>
-      <c r="L46" s="235"/>
-      <c r="M46" s="235"/>
-      <c r="N46" s="235"/>
-      <c r="O46" s="235"/>
-      <c r="P46" s="235"/>
-      <c r="Q46" s="235"/>
-      <c r="R46" s="235"/>
-      <c r="S46" s="235"/>
+      <c r="E46" s="233"/>
+      <c r="F46" s="233"/>
+      <c r="G46" s="233"/>
+      <c r="H46" s="233"/>
+      <c r="I46" s="233"/>
+      <c r="J46" s="233"/>
+      <c r="K46" s="233"/>
+      <c r="L46" s="233"/>
+      <c r="M46" s="233"/>
+      <c r="N46" s="233"/>
+      <c r="O46" s="233"/>
+      <c r="P46" s="233"/>
+      <c r="Q46" s="233"/>
+      <c r="R46" s="233"/>
+      <c r="S46" s="233"/>
     </row>
     <row r="47" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="236"/>
+      <c r="A47" s="229"/>
       <c r="B47" s="24" t="s">
         <v>98</v>
       </c>
       <c r="C47" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="D47" s="235"/>
-      <c r="E47" s="235"/>
-      <c r="F47" s="235"/>
-      <c r="G47" s="235"/>
-      <c r="H47" s="235"/>
-      <c r="I47" s="235"/>
-      <c r="J47" s="235"/>
-      <c r="K47" s="235"/>
-      <c r="L47" s="235"/>
-      <c r="M47" s="235"/>
-      <c r="N47" s="235"/>
-      <c r="O47" s="235"/>
-      <c r="P47" s="235"/>
-      <c r="Q47" s="235"/>
-      <c r="R47" s="235"/>
-      <c r="S47" s="235"/>
+      <c r="D47" s="233"/>
+      <c r="E47" s="233"/>
+      <c r="F47" s="233"/>
+      <c r="G47" s="233"/>
+      <c r="H47" s="233"/>
+      <c r="I47" s="233"/>
+      <c r="J47" s="233"/>
+      <c r="K47" s="233"/>
+      <c r="L47" s="233"/>
+      <c r="M47" s="233"/>
+      <c r="N47" s="233"/>
+      <c r="O47" s="233"/>
+      <c r="P47" s="233"/>
+      <c r="Q47" s="233"/>
+      <c r="R47" s="233"/>
+      <c r="S47" s="233"/>
     </row>
     <row r="48" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="236"/>
+      <c r="A48" s="229"/>
       <c r="B48" s="24" t="s">
         <v>267</v>
       </c>
       <c r="C48" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="D48" s="235"/>
-      <c r="E48" s="235"/>
-      <c r="F48" s="235"/>
-      <c r="G48" s="235"/>
-      <c r="H48" s="235"/>
-      <c r="I48" s="235"/>
-      <c r="J48" s="235"/>
-      <c r="K48" s="235"/>
-      <c r="L48" s="235"/>
-      <c r="M48" s="235"/>
-      <c r="N48" s="235"/>
-      <c r="O48" s="235"/>
-      <c r="P48" s="235"/>
-      <c r="Q48" s="235"/>
-      <c r="R48" s="235"/>
-      <c r="S48" s="235"/>
+      <c r="D48" s="233"/>
+      <c r="E48" s="233"/>
+      <c r="F48" s="233"/>
+      <c r="G48" s="233"/>
+      <c r="H48" s="233"/>
+      <c r="I48" s="233"/>
+      <c r="J48" s="233"/>
+      <c r="K48" s="233"/>
+      <c r="L48" s="233"/>
+      <c r="M48" s="233"/>
+      <c r="N48" s="233"/>
+      <c r="O48" s="233"/>
+      <c r="P48" s="233"/>
+      <c r="Q48" s="233"/>
+      <c r="R48" s="233"/>
+      <c r="S48" s="233"/>
     </row>
     <row r="49" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:19" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A50" s="232" t="s">
+      <c r="A50" s="230" t="s">
         <v>277</v>
       </c>
       <c r="B50" s="115" t="s">
@@ -44177,7 +44177,7 @@
       <c r="S50" s="115"/>
     </row>
     <row r="51" spans="1:19" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="232"/>
+      <c r="A51" s="230"/>
       <c r="B51" s="115" t="s">
         <v>98</v>
       </c>
@@ -44222,7 +44222,7 @@
       <c r="S51" s="115"/>
     </row>
     <row r="52" spans="1:19" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="232"/>
+      <c r="A52" s="230"/>
       <c r="B52" s="115" t="s">
         <v>267</v>
       </c>
@@ -44267,7 +44267,7 @@
       <c r="S52" s="115"/>
     </row>
     <row r="53" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="232"/>
+      <c r="A53" s="230"/>
       <c r="B53" s="180" t="s">
         <v>1430</v>
       </c>
@@ -44290,34 +44290,34 @@
       <c r="S53" s="115"/>
     </row>
     <row r="54" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="232"/>
+      <c r="A54" s="230"/>
       <c r="B54" s="115" t="s">
         <v>40</v>
       </c>
       <c r="C54" s="115" t="s">
         <v>417</v>
       </c>
-      <c r="D54" s="235" t="s">
+      <c r="D54" s="233" t="s">
         <v>1404</v>
       </c>
-      <c r="E54" s="235"/>
-      <c r="F54" s="235"/>
-      <c r="G54" s="235"/>
-      <c r="H54" s="235"/>
-      <c r="I54" s="235"/>
-      <c r="J54" s="235"/>
-      <c r="K54" s="235"/>
-      <c r="L54" s="235"/>
-      <c r="M54" s="235"/>
-      <c r="N54" s="235"/>
-      <c r="O54" s="235"/>
-      <c r="P54" s="235"/>
-      <c r="Q54" s="235"/>
-      <c r="R54" s="235"/>
-      <c r="S54" s="235"/>
+      <c r="E54" s="233"/>
+      <c r="F54" s="233"/>
+      <c r="G54" s="233"/>
+      <c r="H54" s="233"/>
+      <c r="I54" s="233"/>
+      <c r="J54" s="233"/>
+      <c r="K54" s="233"/>
+      <c r="L54" s="233"/>
+      <c r="M54" s="233"/>
+      <c r="N54" s="233"/>
+      <c r="O54" s="233"/>
+      <c r="P54" s="233"/>
+      <c r="Q54" s="233"/>
+      <c r="R54" s="233"/>
+      <c r="S54" s="233"/>
     </row>
     <row r="55" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="232"/>
+      <c r="A55" s="230"/>
       <c r="B55" s="10" t="s">
         <v>278</v>
       </c>
@@ -44351,7 +44351,7 @@
     </row>
     <row r="56" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A57" s="232" t="s">
+      <c r="A57" s="230" t="s">
         <v>279</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -44398,7 +44398,7 @@
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A58" s="232"/>
+      <c r="A58" s="230"/>
       <c r="B58" s="6" t="s">
         <v>98</v>
       </c>
@@ -44443,7 +44443,7 @@
       </c>
     </row>
     <row r="59" spans="1:19" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A59" s="232"/>
+      <c r="A59" s="230"/>
       <c r="B59" s="10" t="s">
         <v>267</v>
       </c>
@@ -44494,7 +44494,7 @@
       </c>
     </row>
     <row r="60" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A60" s="232"/>
+      <c r="A60" s="230"/>
       <c r="B60" s="6" t="s">
         <v>280</v>
       </c>
@@ -44523,7 +44523,7 @@
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A61" s="232"/>
+      <c r="A61" s="230"/>
       <c r="B61" s="6" t="s">
         <v>100</v>
       </c>
@@ -44587,7 +44587,7 @@
       <c r="M62" s="19"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A63" s="232" t="s">
+      <c r="A63" s="230" t="s">
         <v>282</v>
       </c>
       <c r="B63" s="6" t="s">
@@ -44626,7 +44626,7 @@
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A64" s="232"/>
+      <c r="A64" s="230"/>
       <c r="B64" s="6" t="s">
         <v>98</v>
       </c>
@@ -44667,7 +44667,7 @@
       </c>
     </row>
     <row r="65" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A65" s="232"/>
+      <c r="A65" s="230"/>
       <c r="B65" s="6" t="s">
         <v>267</v>
       </c>
@@ -44696,7 +44696,7 @@
       </c>
     </row>
     <row r="66" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A66" s="232"/>
+      <c r="A66" s="230"/>
       <c r="B66" s="6" t="s">
         <v>283</v>
       </c>
@@ -44750,7 +44750,7 @@
       <c r="L67" s="17"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A68" s="232" t="s">
+      <c r="A68" s="230" t="s">
         <v>284</v>
       </c>
       <c r="B68" s="6" t="s">
@@ -44797,7 +44797,7 @@
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A69" s="232"/>
+      <c r="A69" s="230"/>
       <c r="B69" s="6" t="s">
         <v>98</v>
       </c>
@@ -44842,7 +44842,7 @@
       </c>
     </row>
     <row r="70" spans="1:19" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="232"/>
+      <c r="A70" s="230"/>
       <c r="B70" s="6" t="s">
         <v>267</v>
       </c>
@@ -44881,7 +44881,7 @@
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A71" s="232"/>
+      <c r="A71" s="230"/>
       <c r="B71" s="6" t="s">
         <v>137</v>
       </c>
@@ -44926,7 +44926,7 @@
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A72" s="232"/>
+      <c r="A72" s="230"/>
       <c r="B72" s="6" t="s">
         <v>136</v>
       </c>
@@ -44971,7 +44971,7 @@
       </c>
     </row>
     <row r="73" spans="1:19" s="115" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="232"/>
+      <c r="A73" s="230"/>
       <c r="B73" s="10" t="s">
         <v>27</v>
       </c>
@@ -45016,7 +45016,7 @@
       </c>
     </row>
     <row r="74" spans="1:19" s="115" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="232"/>
+      <c r="A74" s="230"/>
       <c r="B74" s="10" t="s">
         <v>52</v>
       </c>
@@ -45061,60 +45061,60 @@
       </c>
     </row>
     <row r="75" spans="1:19" s="181" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="232"/>
+      <c r="A75" s="230"/>
       <c r="B75" s="181" t="s">
         <v>285</v>
       </c>
       <c r="C75" s="182" t="s">
         <v>371</v>
       </c>
-      <c r="D75" s="240" t="s">
+      <c r="D75" s="234" t="s">
         <v>1414</v>
       </c>
-      <c r="E75" s="240"/>
-      <c r="F75" s="240"/>
-      <c r="G75" s="240"/>
-      <c r="H75" s="240"/>
-      <c r="I75" s="240"/>
-      <c r="J75" s="240"/>
-      <c r="K75" s="240"/>
-      <c r="L75" s="240"/>
-      <c r="M75" s="240"/>
-      <c r="N75" s="240"/>
-      <c r="O75" s="240"/>
+      <c r="E75" s="234"/>
+      <c r="F75" s="234"/>
+      <c r="G75" s="234"/>
+      <c r="H75" s="234"/>
+      <c r="I75" s="234"/>
+      <c r="J75" s="234"/>
+      <c r="K75" s="234"/>
+      <c r="L75" s="234"/>
+      <c r="M75" s="234"/>
+      <c r="N75" s="234"/>
+      <c r="O75" s="234"/>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A76" s="232"/>
+      <c r="A76" s="230"/>
       <c r="B76" s="6" t="s">
         <v>286</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="D76" s="235" t="s">
+      <c r="D76" s="233" t="s">
         <v>1415</v>
       </c>
-      <c r="E76" s="235"/>
-      <c r="F76" s="235"/>
-      <c r="G76" s="235"/>
-      <c r="H76" s="235"/>
-      <c r="I76" s="235"/>
-      <c r="J76" s="235"/>
-      <c r="K76" s="235"/>
-      <c r="L76" s="235"/>
-      <c r="M76" s="235"/>
-      <c r="N76" s="235"/>
-      <c r="O76" s="235"/>
-      <c r="P76" s="235"/>
-      <c r="Q76" s="235"/>
-      <c r="R76" s="235"/>
-      <c r="S76" s="235"/>
+      <c r="E76" s="233"/>
+      <c r="F76" s="233"/>
+      <c r="G76" s="233"/>
+      <c r="H76" s="233"/>
+      <c r="I76" s="233"/>
+      <c r="J76" s="233"/>
+      <c r="K76" s="233"/>
+      <c r="L76" s="233"/>
+      <c r="M76" s="233"/>
+      <c r="N76" s="233"/>
+      <c r="O76" s="233"/>
+      <c r="P76" s="233"/>
+      <c r="Q76" s="233"/>
+      <c r="R76" s="233"/>
+      <c r="S76" s="233"/>
     </row>
     <row r="77" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C77" s="17"/>
     </row>
     <row r="78" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="236" t="s">
+      <c r="A78" s="229" t="s">
         <v>287</v>
       </c>
       <c r="B78" s="24" t="s">
@@ -45123,103 +45123,103 @@
       <c r="C78" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D78" s="235" t="s">
+      <c r="D78" s="233" t="s">
         <v>1403</v>
       </c>
-      <c r="E78" s="235"/>
-      <c r="F78" s="235"/>
-      <c r="G78" s="235"/>
-      <c r="H78" s="235"/>
-      <c r="I78" s="235"/>
-      <c r="J78" s="235"/>
-      <c r="K78" s="235"/>
-      <c r="L78" s="235"/>
-      <c r="M78" s="235"/>
-      <c r="N78" s="235"/>
-      <c r="O78" s="235"/>
-      <c r="P78" s="235"/>
-      <c r="Q78" s="235"/>
-      <c r="R78" s="235"/>
-      <c r="S78" s="235"/>
+      <c r="E78" s="233"/>
+      <c r="F78" s="233"/>
+      <c r="G78" s="233"/>
+      <c r="H78" s="233"/>
+      <c r="I78" s="233"/>
+      <c r="J78" s="233"/>
+      <c r="K78" s="233"/>
+      <c r="L78" s="233"/>
+      <c r="M78" s="233"/>
+      <c r="N78" s="233"/>
+      <c r="O78" s="233"/>
+      <c r="P78" s="233"/>
+      <c r="Q78" s="233"/>
+      <c r="R78" s="233"/>
+      <c r="S78" s="233"/>
     </row>
     <row r="79" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="236"/>
+      <c r="A79" s="229"/>
       <c r="B79" s="24" t="s">
         <v>98</v>
       </c>
       <c r="C79" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D79" s="235"/>
-      <c r="E79" s="235"/>
-      <c r="F79" s="235"/>
-      <c r="G79" s="235"/>
-      <c r="H79" s="235"/>
-      <c r="I79" s="235"/>
-      <c r="J79" s="235"/>
-      <c r="K79" s="235"/>
-      <c r="L79" s="235"/>
-      <c r="M79" s="235"/>
-      <c r="N79" s="235"/>
-      <c r="O79" s="235"/>
-      <c r="P79" s="235"/>
-      <c r="Q79" s="235"/>
-      <c r="R79" s="235"/>
-      <c r="S79" s="235"/>
+      <c r="D79" s="233"/>
+      <c r="E79" s="233"/>
+      <c r="F79" s="233"/>
+      <c r="G79" s="233"/>
+      <c r="H79" s="233"/>
+      <c r="I79" s="233"/>
+      <c r="J79" s="233"/>
+      <c r="K79" s="233"/>
+      <c r="L79" s="233"/>
+      <c r="M79" s="233"/>
+      <c r="N79" s="233"/>
+      <c r="O79" s="233"/>
+      <c r="P79" s="233"/>
+      <c r="Q79" s="233"/>
+      <c r="R79" s="233"/>
+      <c r="S79" s="233"/>
     </row>
     <row r="80" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="236"/>
+      <c r="A80" s="229"/>
       <c r="B80" s="24" t="s">
         <v>267</v>
       </c>
       <c r="C80" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D80" s="235"/>
-      <c r="E80" s="235"/>
-      <c r="F80" s="235"/>
-      <c r="G80" s="235"/>
-      <c r="H80" s="235"/>
-      <c r="I80" s="235"/>
-      <c r="J80" s="235"/>
-      <c r="K80" s="235"/>
-      <c r="L80" s="235"/>
-      <c r="M80" s="235"/>
-      <c r="N80" s="235"/>
-      <c r="O80" s="235"/>
-      <c r="P80" s="235"/>
-      <c r="Q80" s="235"/>
-      <c r="R80" s="235"/>
-      <c r="S80" s="235"/>
+      <c r="D80" s="233"/>
+      <c r="E80" s="233"/>
+      <c r="F80" s="233"/>
+      <c r="G80" s="233"/>
+      <c r="H80" s="233"/>
+      <c r="I80" s="233"/>
+      <c r="J80" s="233"/>
+      <c r="K80" s="233"/>
+      <c r="L80" s="233"/>
+      <c r="M80" s="233"/>
+      <c r="N80" s="233"/>
+      <c r="O80" s="233"/>
+      <c r="P80" s="233"/>
+      <c r="Q80" s="233"/>
+      <c r="R80" s="233"/>
+      <c r="S80" s="233"/>
     </row>
     <row r="81" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="236"/>
+      <c r="A81" s="229"/>
       <c r="B81" s="24" t="s">
         <v>288</v>
       </c>
       <c r="C81" s="24" t="s">
         <v>439</v>
       </c>
-      <c r="D81" s="235"/>
-      <c r="E81" s="235"/>
-      <c r="F81" s="235"/>
-      <c r="G81" s="235"/>
-      <c r="H81" s="235"/>
-      <c r="I81" s="235"/>
-      <c r="J81" s="235"/>
-      <c r="K81" s="235"/>
-      <c r="L81" s="235"/>
-      <c r="M81" s="235"/>
-      <c r="N81" s="235"/>
-      <c r="O81" s="235"/>
-      <c r="P81" s="235"/>
-      <c r="Q81" s="235"/>
-      <c r="R81" s="235"/>
-      <c r="S81" s="235"/>
+      <c r="D81" s="233"/>
+      <c r="E81" s="233"/>
+      <c r="F81" s="233"/>
+      <c r="G81" s="233"/>
+      <c r="H81" s="233"/>
+      <c r="I81" s="233"/>
+      <c r="J81" s="233"/>
+      <c r="K81" s="233"/>
+      <c r="L81" s="233"/>
+      <c r="M81" s="233"/>
+      <c r="N81" s="233"/>
+      <c r="O81" s="233"/>
+      <c r="P81" s="233"/>
+      <c r="Q81" s="233"/>
+      <c r="R81" s="233"/>
+      <c r="S81" s="233"/>
     </row>
     <row r="82" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="83" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="236" t="s">
+      <c r="A83" s="229" t="s">
         <v>289</v>
       </c>
       <c r="B83" s="24" t="s">
@@ -45228,103 +45228,103 @@
       <c r="C83" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D83" s="235" t="s">
+      <c r="D83" s="233" t="s">
         <v>1416</v>
       </c>
-      <c r="E83" s="235"/>
-      <c r="F83" s="235"/>
-      <c r="G83" s="235"/>
-      <c r="H83" s="235"/>
-      <c r="I83" s="235"/>
-      <c r="J83" s="235"/>
-      <c r="K83" s="235"/>
-      <c r="L83" s="235"/>
-      <c r="M83" s="235"/>
-      <c r="N83" s="235"/>
-      <c r="O83" s="235"/>
-      <c r="P83" s="235"/>
-      <c r="Q83" s="235"/>
-      <c r="R83" s="235"/>
-      <c r="S83" s="235"/>
+      <c r="E83" s="233"/>
+      <c r="F83" s="233"/>
+      <c r="G83" s="233"/>
+      <c r="H83" s="233"/>
+      <c r="I83" s="233"/>
+      <c r="J83" s="233"/>
+      <c r="K83" s="233"/>
+      <c r="L83" s="233"/>
+      <c r="M83" s="233"/>
+      <c r="N83" s="233"/>
+      <c r="O83" s="233"/>
+      <c r="P83" s="233"/>
+      <c r="Q83" s="233"/>
+      <c r="R83" s="233"/>
+      <c r="S83" s="233"/>
     </row>
     <row r="84" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="236"/>
+      <c r="A84" s="229"/>
       <c r="B84" s="24" t="s">
         <v>98</v>
       </c>
       <c r="C84" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D84" s="235"/>
-      <c r="E84" s="235"/>
-      <c r="F84" s="235"/>
-      <c r="G84" s="235"/>
-      <c r="H84" s="235"/>
-      <c r="I84" s="235"/>
-      <c r="J84" s="235"/>
-      <c r="K84" s="235"/>
-      <c r="L84" s="235"/>
-      <c r="M84" s="235"/>
-      <c r="N84" s="235"/>
-      <c r="O84" s="235"/>
-      <c r="P84" s="235"/>
-      <c r="Q84" s="235"/>
-      <c r="R84" s="235"/>
-      <c r="S84" s="235"/>
+      <c r="D84" s="233"/>
+      <c r="E84" s="233"/>
+      <c r="F84" s="233"/>
+      <c r="G84" s="233"/>
+      <c r="H84" s="233"/>
+      <c r="I84" s="233"/>
+      <c r="J84" s="233"/>
+      <c r="K84" s="233"/>
+      <c r="L84" s="233"/>
+      <c r="M84" s="233"/>
+      <c r="N84" s="233"/>
+      <c r="O84" s="233"/>
+      <c r="P84" s="233"/>
+      <c r="Q84" s="233"/>
+      <c r="R84" s="233"/>
+      <c r="S84" s="233"/>
     </row>
     <row r="85" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="236"/>
+      <c r="A85" s="229"/>
       <c r="B85" s="24" t="s">
         <v>290</v>
       </c>
       <c r="C85" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D85" s="235"/>
-      <c r="E85" s="235"/>
-      <c r="F85" s="235"/>
-      <c r="G85" s="235"/>
-      <c r="H85" s="235"/>
-      <c r="I85" s="235"/>
-      <c r="J85" s="235"/>
-      <c r="K85" s="235"/>
-      <c r="L85" s="235"/>
-      <c r="M85" s="235"/>
-      <c r="N85" s="235"/>
-      <c r="O85" s="235"/>
-      <c r="P85" s="235"/>
-      <c r="Q85" s="235"/>
-      <c r="R85" s="235"/>
-      <c r="S85" s="235"/>
+      <c r="D85" s="233"/>
+      <c r="E85" s="233"/>
+      <c r="F85" s="233"/>
+      <c r="G85" s="233"/>
+      <c r="H85" s="233"/>
+      <c r="I85" s="233"/>
+      <c r="J85" s="233"/>
+      <c r="K85" s="233"/>
+      <c r="L85" s="233"/>
+      <c r="M85" s="233"/>
+      <c r="N85" s="233"/>
+      <c r="O85" s="233"/>
+      <c r="P85" s="233"/>
+      <c r="Q85" s="233"/>
+      <c r="R85" s="233"/>
+      <c r="S85" s="233"/>
     </row>
     <row r="86" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="236"/>
+      <c r="A86" s="229"/>
       <c r="B86" s="24" t="s">
         <v>291</v>
       </c>
       <c r="C86" s="24" t="s">
         <v>440</v>
       </c>
-      <c r="D86" s="235"/>
-      <c r="E86" s="235"/>
-      <c r="F86" s="235"/>
-      <c r="G86" s="235"/>
-      <c r="H86" s="235"/>
-      <c r="I86" s="235"/>
-      <c r="J86" s="235"/>
-      <c r="K86" s="235"/>
-      <c r="L86" s="235"/>
-      <c r="M86" s="235"/>
-      <c r="N86" s="235"/>
-      <c r="O86" s="235"/>
-      <c r="P86" s="235"/>
-      <c r="Q86" s="235"/>
-      <c r="R86" s="235"/>
-      <c r="S86" s="235"/>
+      <c r="D86" s="233"/>
+      <c r="E86" s="233"/>
+      <c r="F86" s="233"/>
+      <c r="G86" s="233"/>
+      <c r="H86" s="233"/>
+      <c r="I86" s="233"/>
+      <c r="J86" s="233"/>
+      <c r="K86" s="233"/>
+      <c r="L86" s="233"/>
+      <c r="M86" s="233"/>
+      <c r="N86" s="233"/>
+      <c r="O86" s="233"/>
+      <c r="P86" s="233"/>
+      <c r="Q86" s="233"/>
+      <c r="R86" s="233"/>
+      <c r="S86" s="233"/>
     </row>
     <row r="87" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="88" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="236" t="s">
+      <c r="A88" s="229" t="s">
         <v>292</v>
       </c>
       <c r="B88" s="24" t="s">
@@ -45333,253 +45333,253 @@
       <c r="C88" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D88" s="235" t="s">
+      <c r="D88" s="233" t="s">
         <v>1417</v>
       </c>
-      <c r="E88" s="235"/>
-      <c r="F88" s="235"/>
-      <c r="G88" s="235"/>
-      <c r="H88" s="235"/>
-      <c r="I88" s="235"/>
-      <c r="J88" s="235"/>
-      <c r="K88" s="235"/>
-      <c r="L88" s="235"/>
-      <c r="M88" s="235"/>
-      <c r="N88" s="235"/>
-      <c r="O88" s="235"/>
-      <c r="P88" s="235"/>
-      <c r="Q88" s="235"/>
-      <c r="R88" s="235"/>
-      <c r="S88" s="235"/>
+      <c r="E88" s="233"/>
+      <c r="F88" s="233"/>
+      <c r="G88" s="233"/>
+      <c r="H88" s="233"/>
+      <c r="I88" s="233"/>
+      <c r="J88" s="233"/>
+      <c r="K88" s="233"/>
+      <c r="L88" s="233"/>
+      <c r="M88" s="233"/>
+      <c r="N88" s="233"/>
+      <c r="O88" s="233"/>
+      <c r="P88" s="233"/>
+      <c r="Q88" s="233"/>
+      <c r="R88" s="233"/>
+      <c r="S88" s="233"/>
     </row>
     <row r="89" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="236"/>
+      <c r="A89" s="229"/>
       <c r="B89" s="24" t="s">
         <v>98</v>
       </c>
       <c r="C89" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D89" s="235"/>
-      <c r="E89" s="235"/>
-      <c r="F89" s="235"/>
-      <c r="G89" s="235"/>
-      <c r="H89" s="235"/>
-      <c r="I89" s="235"/>
-      <c r="J89" s="235"/>
-      <c r="K89" s="235"/>
-      <c r="L89" s="235"/>
-      <c r="M89" s="235"/>
-      <c r="N89" s="235"/>
-      <c r="O89" s="235"/>
-      <c r="P89" s="235"/>
-      <c r="Q89" s="235"/>
-      <c r="R89" s="235"/>
-      <c r="S89" s="235"/>
+      <c r="D89" s="233"/>
+      <c r="E89" s="233"/>
+      <c r="F89" s="233"/>
+      <c r="G89" s="233"/>
+      <c r="H89" s="233"/>
+      <c r="I89" s="233"/>
+      <c r="J89" s="233"/>
+      <c r="K89" s="233"/>
+      <c r="L89" s="233"/>
+      <c r="M89" s="233"/>
+      <c r="N89" s="233"/>
+      <c r="O89" s="233"/>
+      <c r="P89" s="233"/>
+      <c r="Q89" s="233"/>
+      <c r="R89" s="233"/>
+      <c r="S89" s="233"/>
     </row>
     <row r="90" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="236"/>
+      <c r="A90" s="229"/>
       <c r="B90" s="24" t="s">
         <v>267</v>
       </c>
       <c r="C90" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="D90" s="235"/>
-      <c r="E90" s="235"/>
-      <c r="F90" s="235"/>
-      <c r="G90" s="235"/>
-      <c r="H90" s="235"/>
-      <c r="I90" s="235"/>
-      <c r="J90" s="235"/>
-      <c r="K90" s="235"/>
-      <c r="L90" s="235"/>
-      <c r="M90" s="235"/>
-      <c r="N90" s="235"/>
-      <c r="O90" s="235"/>
-      <c r="P90" s="235"/>
-      <c r="Q90" s="235"/>
-      <c r="R90" s="235"/>
-      <c r="S90" s="235"/>
+      <c r="D90" s="233"/>
+      <c r="E90" s="233"/>
+      <c r="F90" s="233"/>
+      <c r="G90" s="233"/>
+      <c r="H90" s="233"/>
+      <c r="I90" s="233"/>
+      <c r="J90" s="233"/>
+      <c r="K90" s="233"/>
+      <c r="L90" s="233"/>
+      <c r="M90" s="233"/>
+      <c r="N90" s="233"/>
+      <c r="O90" s="233"/>
+      <c r="P90" s="233"/>
+      <c r="Q90" s="233"/>
+      <c r="R90" s="233"/>
+      <c r="S90" s="233"/>
     </row>
     <row r="91" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="236"/>
+      <c r="A91" s="229"/>
       <c r="B91" s="24" t="s">
         <v>137</v>
       </c>
       <c r="C91" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="D91" s="235"/>
-      <c r="E91" s="235"/>
-      <c r="F91" s="235"/>
-      <c r="G91" s="235"/>
-      <c r="H91" s="235"/>
-      <c r="I91" s="235"/>
-      <c r="J91" s="235"/>
-      <c r="K91" s="235"/>
-      <c r="L91" s="235"/>
-      <c r="M91" s="235"/>
-      <c r="N91" s="235"/>
-      <c r="O91" s="235"/>
-      <c r="P91" s="235"/>
-      <c r="Q91" s="235"/>
-      <c r="R91" s="235"/>
-      <c r="S91" s="235"/>
+      <c r="D91" s="233"/>
+      <c r="E91" s="233"/>
+      <c r="F91" s="233"/>
+      <c r="G91" s="233"/>
+      <c r="H91" s="233"/>
+      <c r="I91" s="233"/>
+      <c r="J91" s="233"/>
+      <c r="K91" s="233"/>
+      <c r="L91" s="233"/>
+      <c r="M91" s="233"/>
+      <c r="N91" s="233"/>
+      <c r="O91" s="233"/>
+      <c r="P91" s="233"/>
+      <c r="Q91" s="233"/>
+      <c r="R91" s="233"/>
+      <c r="S91" s="233"/>
     </row>
     <row r="92" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="236"/>
+      <c r="A92" s="229"/>
       <c r="B92" s="24" t="s">
         <v>136</v>
       </c>
       <c r="C92" s="24" t="s">
         <v>331</v>
       </c>
-      <c r="D92" s="235"/>
-      <c r="E92" s="235"/>
-      <c r="F92" s="235"/>
-      <c r="G92" s="235"/>
-      <c r="H92" s="235"/>
-      <c r="I92" s="235"/>
-      <c r="J92" s="235"/>
-      <c r="K92" s="235"/>
-      <c r="L92" s="235"/>
-      <c r="M92" s="235"/>
-      <c r="N92" s="235"/>
-      <c r="O92" s="235"/>
-      <c r="P92" s="235"/>
-      <c r="Q92" s="235"/>
-      <c r="R92" s="235"/>
-      <c r="S92" s="235"/>
+      <c r="D92" s="233"/>
+      <c r="E92" s="233"/>
+      <c r="F92" s="233"/>
+      <c r="G92" s="233"/>
+      <c r="H92" s="233"/>
+      <c r="I92" s="233"/>
+      <c r="J92" s="233"/>
+      <c r="K92" s="233"/>
+      <c r="L92" s="233"/>
+      <c r="M92" s="233"/>
+      <c r="N92" s="233"/>
+      <c r="O92" s="233"/>
+      <c r="P92" s="233"/>
+      <c r="Q92" s="233"/>
+      <c r="R92" s="233"/>
+      <c r="S92" s="233"/>
     </row>
     <row r="93" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="236"/>
+      <c r="A93" s="229"/>
       <c r="B93" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C93" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="D93" s="235"/>
-      <c r="E93" s="235"/>
-      <c r="F93" s="235"/>
-      <c r="G93" s="235"/>
-      <c r="H93" s="235"/>
-      <c r="I93" s="235"/>
-      <c r="J93" s="235"/>
-      <c r="K93" s="235"/>
-      <c r="L93" s="235"/>
-      <c r="M93" s="235"/>
-      <c r="N93" s="235"/>
-      <c r="O93" s="235"/>
-      <c r="P93" s="235"/>
-      <c r="Q93" s="235"/>
-      <c r="R93" s="235"/>
-      <c r="S93" s="235"/>
+      <c r="D93" s="233"/>
+      <c r="E93" s="233"/>
+      <c r="F93" s="233"/>
+      <c r="G93" s="233"/>
+      <c r="H93" s="233"/>
+      <c r="I93" s="233"/>
+      <c r="J93" s="233"/>
+      <c r="K93" s="233"/>
+      <c r="L93" s="233"/>
+      <c r="M93" s="233"/>
+      <c r="N93" s="233"/>
+      <c r="O93" s="233"/>
+      <c r="P93" s="233"/>
+      <c r="Q93" s="233"/>
+      <c r="R93" s="233"/>
+      <c r="S93" s="233"/>
     </row>
     <row r="94" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="236"/>
+      <c r="A94" s="229"/>
       <c r="B94" s="27" t="s">
         <v>52</v>
       </c>
       <c r="C94" s="27" t="s">
         <v>331</v>
       </c>
-      <c r="D94" s="235"/>
-      <c r="E94" s="235"/>
-      <c r="F94" s="235"/>
-      <c r="G94" s="235"/>
-      <c r="H94" s="235"/>
-      <c r="I94" s="235"/>
-      <c r="J94" s="235"/>
-      <c r="K94" s="235"/>
-      <c r="L94" s="235"/>
-      <c r="M94" s="235"/>
-      <c r="N94" s="235"/>
-      <c r="O94" s="235"/>
-      <c r="P94" s="235"/>
-      <c r="Q94" s="235"/>
-      <c r="R94" s="235"/>
-      <c r="S94" s="235"/>
+      <c r="D94" s="233"/>
+      <c r="E94" s="233"/>
+      <c r="F94" s="233"/>
+      <c r="G94" s="233"/>
+      <c r="H94" s="233"/>
+      <c r="I94" s="233"/>
+      <c r="J94" s="233"/>
+      <c r="K94" s="233"/>
+      <c r="L94" s="233"/>
+      <c r="M94" s="233"/>
+      <c r="N94" s="233"/>
+      <c r="O94" s="233"/>
+      <c r="P94" s="233"/>
+      <c r="Q94" s="233"/>
+      <c r="R94" s="233"/>
+      <c r="S94" s="233"/>
     </row>
     <row r="95" spans="1:19" s="181" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="236"/>
+      <c r="A95" s="229"/>
       <c r="B95" s="181" t="s">
         <v>285</v>
       </c>
       <c r="C95" s="181" t="s">
         <v>371</v>
       </c>
-      <c r="D95" s="235"/>
-      <c r="E95" s="235"/>
-      <c r="F95" s="235"/>
-      <c r="G95" s="235"/>
-      <c r="H95" s="235"/>
-      <c r="I95" s="235"/>
-      <c r="J95" s="235"/>
-      <c r="K95" s="235"/>
-      <c r="L95" s="235"/>
-      <c r="M95" s="235"/>
-      <c r="N95" s="235"/>
-      <c r="O95" s="235"/>
-      <c r="P95" s="235"/>
-      <c r="Q95" s="235"/>
-      <c r="R95" s="235"/>
-      <c r="S95" s="235"/>
+      <c r="D95" s="233"/>
+      <c r="E95" s="233"/>
+      <c r="F95" s="233"/>
+      <c r="G95" s="233"/>
+      <c r="H95" s="233"/>
+      <c r="I95" s="233"/>
+      <c r="J95" s="233"/>
+      <c r="K95" s="233"/>
+      <c r="L95" s="233"/>
+      <c r="M95" s="233"/>
+      <c r="N95" s="233"/>
+      <c r="O95" s="233"/>
+      <c r="P95" s="233"/>
+      <c r="Q95" s="233"/>
+      <c r="R95" s="233"/>
+      <c r="S95" s="233"/>
     </row>
     <row r="96" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="236"/>
+      <c r="A96" s="229"/>
       <c r="B96" s="24" t="s">
         <v>286</v>
       </c>
       <c r="C96" s="24" t="s">
         <v>272</v>
       </c>
-      <c r="D96" s="235"/>
-      <c r="E96" s="235"/>
-      <c r="F96" s="235"/>
-      <c r="G96" s="235"/>
-      <c r="H96" s="235"/>
-      <c r="I96" s="235"/>
-      <c r="J96" s="235"/>
-      <c r="K96" s="235"/>
-      <c r="L96" s="235"/>
-      <c r="M96" s="235"/>
-      <c r="N96" s="235"/>
-      <c r="O96" s="235"/>
-      <c r="P96" s="235"/>
-      <c r="Q96" s="235"/>
-      <c r="R96" s="235"/>
-      <c r="S96" s="235"/>
+      <c r="D96" s="233"/>
+      <c r="E96" s="233"/>
+      <c r="F96" s="233"/>
+      <c r="G96" s="233"/>
+      <c r="H96" s="233"/>
+      <c r="I96" s="233"/>
+      <c r="J96" s="233"/>
+      <c r="K96" s="233"/>
+      <c r="L96" s="233"/>
+      <c r="M96" s="233"/>
+      <c r="N96" s="233"/>
+      <c r="O96" s="233"/>
+      <c r="P96" s="233"/>
+      <c r="Q96" s="233"/>
+      <c r="R96" s="233"/>
+      <c r="S96" s="233"/>
     </row>
     <row r="97" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="236"/>
+      <c r="A97" s="229"/>
       <c r="B97" s="24" t="s">
         <v>256</v>
       </c>
       <c r="C97" s="24" t="s">
         <v>287</v>
       </c>
-      <c r="D97" s="235"/>
-      <c r="E97" s="235"/>
-      <c r="F97" s="235"/>
-      <c r="G97" s="235"/>
-      <c r="H97" s="235"/>
-      <c r="I97" s="235"/>
-      <c r="J97" s="235"/>
-      <c r="K97" s="235"/>
-      <c r="L97" s="235"/>
-      <c r="M97" s="235"/>
-      <c r="N97" s="235"/>
-      <c r="O97" s="235"/>
-      <c r="P97" s="235"/>
-      <c r="Q97" s="235"/>
-      <c r="R97" s="235"/>
-      <c r="S97" s="235"/>
+      <c r="D97" s="233"/>
+      <c r="E97" s="233"/>
+      <c r="F97" s="233"/>
+      <c r="G97" s="233"/>
+      <c r="H97" s="233"/>
+      <c r="I97" s="233"/>
+      <c r="J97" s="233"/>
+      <c r="K97" s="233"/>
+      <c r="L97" s="233"/>
+      <c r="M97" s="233"/>
+      <c r="N97" s="233"/>
+      <c r="O97" s="233"/>
+      <c r="P97" s="233"/>
+      <c r="Q97" s="233"/>
+      <c r="R97" s="233"/>
+      <c r="S97" s="233"/>
     </row>
     <row r="98" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="99" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A99" s="232" t="s">
+      <c r="A99" s="230" t="s">
         <v>293</v>
       </c>
       <c r="B99" s="24" t="s">
@@ -45607,7 +45607,7 @@
       <c r="T99" s="24"/>
     </row>
     <row r="100" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="232"/>
+      <c r="A100" s="230"/>
       <c r="B100" s="24" t="s">
         <v>98</v>
       </c>
@@ -45635,7 +45635,7 @@
       <c r="T100" s="24"/>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A101" s="232"/>
+      <c r="A101" s="230"/>
       <c r="B101" s="24" t="s">
         <v>267</v>
       </c>
@@ -45663,7 +45663,7 @@
       <c r="T101" s="24"/>
     </row>
     <row r="102" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A102" s="232"/>
+      <c r="A102" s="230"/>
       <c r="B102" s="6" t="s">
         <v>137</v>
       </c>
@@ -45708,7 +45708,7 @@
       </c>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A103" s="232"/>
+      <c r="A103" s="230"/>
       <c r="B103" s="24" t="s">
         <v>136</v>
       </c>
@@ -45736,7 +45736,7 @@
       <c r="T103" s="8"/>
     </row>
     <row r="104" spans="1:20" s="181" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="232"/>
+      <c r="A104" s="230"/>
       <c r="B104" s="181" t="s">
         <v>285</v>
       </c>
@@ -45748,101 +45748,101 @@
       </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A105" s="232"/>
+      <c r="A105" s="230"/>
       <c r="B105" s="24" t="s">
         <v>294</v>
       </c>
       <c r="C105" s="24" t="s">
         <v>438</v>
       </c>
-      <c r="D105" s="235" t="s">
+      <c r="D105" s="233" t="s">
         <v>1420</v>
       </c>
-      <c r="E105" s="235"/>
-      <c r="F105" s="235"/>
-      <c r="G105" s="235"/>
-      <c r="H105" s="235"/>
-      <c r="I105" s="235"/>
-      <c r="J105" s="235"/>
-      <c r="K105" s="235"/>
-      <c r="L105" s="235"/>
-      <c r="M105" s="235"/>
-      <c r="N105" s="235"/>
-      <c r="O105" s="235"/>
-      <c r="P105" s="235"/>
-      <c r="Q105" s="235"/>
-      <c r="R105" s="235"/>
-      <c r="S105" s="235"/>
+      <c r="E105" s="233"/>
+      <c r="F105" s="233"/>
+      <c r="G105" s="233"/>
+      <c r="H105" s="233"/>
+      <c r="I105" s="233"/>
+      <c r="J105" s="233"/>
+      <c r="K105" s="233"/>
+      <c r="L105" s="233"/>
+      <c r="M105" s="233"/>
+      <c r="N105" s="233"/>
+      <c r="O105" s="233"/>
+      <c r="P105" s="233"/>
+      <c r="Q105" s="233"/>
+      <c r="R105" s="233"/>
+      <c r="S105" s="233"/>
       <c r="T105" s="24"/>
     </row>
     <row r="106" spans="1:20" s="181" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="232"/>
+      <c r="A106" s="230"/>
       <c r="B106" s="181" t="s">
         <v>295</v>
       </c>
       <c r="C106" s="182" t="s">
         <v>373</v>
       </c>
-      <c r="D106" s="231" t="s">
+      <c r="D106" s="240" t="s">
         <v>1070</v>
       </c>
-      <c r="E106" s="231" t="s">
+      <c r="E106" s="240" t="s">
         <v>587</v>
       </c>
-      <c r="F106" s="231" t="s">
+      <c r="F106" s="240" t="s">
         <v>1070</v>
       </c>
-      <c r="G106" s="231" t="s">
+      <c r="G106" s="240" t="s">
         <v>587</v>
       </c>
-      <c r="H106" s="231" t="s">
+      <c r="H106" s="240" t="s">
         <v>377</v>
       </c>
-      <c r="I106" s="231" t="s">
+      <c r="I106" s="240" t="s">
         <v>376</v>
       </c>
-      <c r="J106" s="231" t="s">
+      <c r="J106" s="240" t="s">
         <v>378</v>
       </c>
-      <c r="K106" s="231" t="s">
+      <c r="K106" s="240" t="s">
         <v>372</v>
       </c>
-      <c r="L106" s="229" t="s">
+      <c r="L106" s="238" t="s">
         <v>1071</v>
       </c>
-      <c r="M106" s="229" t="s">
+      <c r="M106" s="238" t="s">
         <v>1072</v>
       </c>
-      <c r="N106" s="230" t="s">
+      <c r="N106" s="239" t="s">
         <v>504</v>
       </c>
-      <c r="O106" s="230" t="s">
+      <c r="O106" s="239" t="s">
         <v>1073</v>
       </c>
     </row>
     <row r="107" spans="1:20" s="181" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="232"/>
+      <c r="A107" s="230"/>
       <c r="B107" s="181" t="s">
         <v>296</v>
       </c>
       <c r="C107" s="182" t="s">
         <v>374</v>
       </c>
-      <c r="D107" s="231"/>
-      <c r="E107" s="231"/>
-      <c r="F107" s="231"/>
-      <c r="G107" s="231"/>
-      <c r="H107" s="231"/>
-      <c r="I107" s="231"/>
-      <c r="J107" s="231"/>
-      <c r="K107" s="231"/>
-      <c r="L107" s="229"/>
-      <c r="M107" s="229"/>
-      <c r="N107" s="230"/>
-      <c r="O107" s="230"/>
+      <c r="D107" s="240"/>
+      <c r="E107" s="240"/>
+      <c r="F107" s="240"/>
+      <c r="G107" s="240"/>
+      <c r="H107" s="240"/>
+      <c r="I107" s="240"/>
+      <c r="J107" s="240"/>
+      <c r="K107" s="240"/>
+      <c r="L107" s="238"/>
+      <c r="M107" s="238"/>
+      <c r="N107" s="239"/>
+      <c r="O107" s="239"/>
     </row>
     <row r="108" spans="1:20" s="115" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="232"/>
+      <c r="A108" s="230"/>
       <c r="B108" s="115" t="s">
         <v>139</v>
       </c>
@@ -45877,7 +45877,7 @@
       </c>
     </row>
     <row r="109" spans="1:20" s="115" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="232"/>
+      <c r="A109" s="230"/>
       <c r="B109" s="10" t="s">
         <v>268</v>
       </c>
@@ -45905,7 +45905,7 @@
       <c r="K110" s="20"/>
     </row>
     <row r="111" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="238" t="s">
+      <c r="A111" s="236" t="s">
         <v>297</v>
       </c>
       <c r="B111" s="8" t="s">
@@ -45940,7 +45940,7 @@
       </c>
     </row>
     <row r="112" spans="1:20" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A112" s="238"/>
+      <c r="A112" s="236"/>
       <c r="B112" s="8" t="s">
         <v>98</v>
       </c>
@@ -45979,7 +45979,7 @@
       </c>
     </row>
     <row r="113" spans="1:20" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A113" s="238"/>
+      <c r="A113" s="236"/>
       <c r="B113" s="8" t="s">
         <v>267</v>
       </c>
@@ -46006,7 +46006,7 @@
       </c>
     </row>
     <row r="114" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="238"/>
+      <c r="A114" s="236"/>
       <c r="B114" s="8" t="s">
         <v>298</v>
       </c>
@@ -46036,7 +46036,7 @@
       <c r="C115" s="17"/>
     </row>
     <row r="116" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="238" t="s">
+      <c r="A116" s="236" t="s">
         <v>517</v>
       </c>
       <c r="B116" s="28" t="s">
@@ -46045,18 +46045,18 @@
       <c r="C116" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="D116" s="235" t="s">
+      <c r="D116" s="233" t="s">
         <v>1421</v>
       </c>
-      <c r="E116" s="235"/>
-      <c r="F116" s="235"/>
-      <c r="G116" s="235"/>
-      <c r="H116" s="235"/>
-      <c r="I116" s="235"/>
-      <c r="J116" s="235"/>
-      <c r="K116" s="235"/>
-      <c r="L116" s="235"/>
-      <c r="M116" s="235"/>
+      <c r="E116" s="233"/>
+      <c r="F116" s="233"/>
+      <c r="G116" s="233"/>
+      <c r="H116" s="233"/>
+      <c r="I116" s="233"/>
+      <c r="J116" s="233"/>
+      <c r="K116" s="233"/>
+      <c r="L116" s="233"/>
+      <c r="M116" s="233"/>
       <c r="N116" s="8" t="s">
         <v>519</v>
       </c>
@@ -46065,23 +46065,23 @@
       </c>
     </row>
     <row r="117" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="238"/>
+      <c r="A117" s="236"/>
       <c r="B117" s="28" t="s">
         <v>98</v>
       </c>
       <c r="C117" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="D117" s="235"/>
-      <c r="E117" s="235"/>
-      <c r="F117" s="235"/>
-      <c r="G117" s="235"/>
-      <c r="H117" s="235"/>
-      <c r="I117" s="235"/>
-      <c r="J117" s="235"/>
-      <c r="K117" s="235"/>
-      <c r="L117" s="235"/>
-      <c r="M117" s="235"/>
+      <c r="D117" s="233"/>
+      <c r="E117" s="233"/>
+      <c r="F117" s="233"/>
+      <c r="G117" s="233"/>
+      <c r="H117" s="233"/>
+      <c r="I117" s="233"/>
+      <c r="J117" s="233"/>
+      <c r="K117" s="233"/>
+      <c r="L117" s="233"/>
+      <c r="M117" s="233"/>
       <c r="N117" s="8" t="s">
         <v>520</v>
       </c>
@@ -46090,23 +46090,23 @@
       </c>
     </row>
     <row r="118" spans="1:20" s="8" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A118" s="238"/>
+      <c r="A118" s="236"/>
       <c r="B118" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C118" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="D118" s="235"/>
-      <c r="E118" s="235"/>
-      <c r="F118" s="235"/>
-      <c r="G118" s="235"/>
-      <c r="H118" s="235"/>
-      <c r="I118" s="235"/>
-      <c r="J118" s="235"/>
-      <c r="K118" s="235"/>
-      <c r="L118" s="235"/>
-      <c r="M118" s="235"/>
+      <c r="D118" s="233"/>
+      <c r="E118" s="233"/>
+      <c r="F118" s="233"/>
+      <c r="G118" s="233"/>
+      <c r="H118" s="233"/>
+      <c r="I118" s="233"/>
+      <c r="J118" s="233"/>
+      <c r="K118" s="233"/>
+      <c r="L118" s="233"/>
+      <c r="M118" s="233"/>
       <c r="N118" s="173" t="s">
         <v>1382</v>
       </c>
@@ -46115,46 +46115,46 @@
       </c>
     </row>
     <row r="119" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="238"/>
+      <c r="A119" s="236"/>
       <c r="B119" s="28" t="s">
         <v>22</v>
       </c>
       <c r="C119" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="D119" s="235"/>
-      <c r="E119" s="235"/>
-      <c r="F119" s="235"/>
-      <c r="G119" s="235"/>
-      <c r="H119" s="235"/>
-      <c r="I119" s="235"/>
-      <c r="J119" s="235"/>
-      <c r="K119" s="235"/>
-      <c r="L119" s="235"/>
-      <c r="M119" s="235"/>
-      <c r="N119" s="235" t="s">
+      <c r="D119" s="233"/>
+      <c r="E119" s="233"/>
+      <c r="F119" s="233"/>
+      <c r="G119" s="233"/>
+      <c r="H119" s="233"/>
+      <c r="I119" s="233"/>
+      <c r="J119" s="233"/>
+      <c r="K119" s="233"/>
+      <c r="L119" s="233"/>
+      <c r="M119" s="233"/>
+      <c r="N119" s="233" t="s">
         <v>1422</v>
       </c>
-      <c r="O119" s="235"/>
+      <c r="O119" s="233"/>
     </row>
     <row r="120" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="238"/>
+      <c r="A120" s="236"/>
       <c r="B120" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C120" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="D120" s="235"/>
-      <c r="E120" s="235"/>
-      <c r="F120" s="235"/>
-      <c r="G120" s="235"/>
-      <c r="H120" s="235"/>
-      <c r="I120" s="235"/>
-      <c r="J120" s="235"/>
-      <c r="K120" s="235"/>
-      <c r="L120" s="235"/>
-      <c r="M120" s="235"/>
+      <c r="D120" s="233"/>
+      <c r="E120" s="233"/>
+      <c r="F120" s="233"/>
+      <c r="G120" s="233"/>
+      <c r="H120" s="233"/>
+      <c r="I120" s="233"/>
+      <c r="J120" s="233"/>
+      <c r="K120" s="233"/>
+      <c r="L120" s="233"/>
+      <c r="M120" s="233"/>
       <c r="N120" s="8" t="s">
         <v>1381</v>
       </c>
@@ -46163,89 +46163,89 @@
       </c>
     </row>
     <row r="121" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="238"/>
+      <c r="A121" s="236"/>
       <c r="B121" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C121" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="D121" s="235"/>
-      <c r="E121" s="235"/>
-      <c r="F121" s="235"/>
-      <c r="G121" s="235"/>
-      <c r="H121" s="235"/>
-      <c r="I121" s="235"/>
-      <c r="J121" s="235"/>
-      <c r="K121" s="235"/>
-      <c r="L121" s="235"/>
-      <c r="M121" s="235"/>
-      <c r="N121" s="235" t="s">
+      <c r="D121" s="233"/>
+      <c r="E121" s="233"/>
+      <c r="F121" s="233"/>
+      <c r="G121" s="233"/>
+      <c r="H121" s="233"/>
+      <c r="I121" s="233"/>
+      <c r="J121" s="233"/>
+      <c r="K121" s="233"/>
+      <c r="L121" s="233"/>
+      <c r="M121" s="233"/>
+      <c r="N121" s="233" t="s">
         <v>1422</v>
       </c>
-      <c r="O121" s="235"/>
+      <c r="O121" s="233"/>
     </row>
     <row r="122" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="238"/>
+      <c r="A122" s="236"/>
       <c r="B122" s="10" t="s">
         <v>390</v>
       </c>
       <c r="C122" s="10" t="s">
         <v>391</v>
       </c>
-      <c r="D122" s="235"/>
-      <c r="E122" s="235"/>
-      <c r="F122" s="235"/>
-      <c r="G122" s="235"/>
-      <c r="H122" s="235"/>
-      <c r="I122" s="235"/>
-      <c r="J122" s="235"/>
-      <c r="K122" s="235"/>
-      <c r="L122" s="235"/>
-      <c r="M122" s="235"/>
-      <c r="N122" s="235"/>
-      <c r="O122" s="235"/>
+      <c r="D122" s="233"/>
+      <c r="E122" s="233"/>
+      <c r="F122" s="233"/>
+      <c r="G122" s="233"/>
+      <c r="H122" s="233"/>
+      <c r="I122" s="233"/>
+      <c r="J122" s="233"/>
+      <c r="K122" s="233"/>
+      <c r="L122" s="233"/>
+      <c r="M122" s="233"/>
+      <c r="N122" s="233"/>
+      <c r="O122" s="233"/>
     </row>
     <row r="123" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="238"/>
+      <c r="A123" s="236"/>
       <c r="B123" s="28" t="s">
         <v>273</v>
       </c>
       <c r="C123" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D123" s="235"/>
-      <c r="E123" s="235"/>
-      <c r="F123" s="235"/>
-      <c r="G123" s="235"/>
-      <c r="H123" s="235"/>
-      <c r="I123" s="235"/>
-      <c r="J123" s="235"/>
-      <c r="K123" s="235"/>
-      <c r="L123" s="235"/>
-      <c r="M123" s="235"/>
+      <c r="D123" s="233"/>
+      <c r="E123" s="233"/>
+      <c r="F123" s="233"/>
+      <c r="G123" s="233"/>
+      <c r="H123" s="233"/>
+      <c r="I123" s="233"/>
+      <c r="J123" s="233"/>
+      <c r="K123" s="233"/>
+      <c r="L123" s="233"/>
+      <c r="M123" s="233"/>
       <c r="N123" s="8" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="124" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="238"/>
+      <c r="A124" s="236"/>
       <c r="B124" s="28" t="s">
         <v>274</v>
       </c>
       <c r="C124" s="10" t="s">
         <v>437</v>
       </c>
-      <c r="D124" s="235"/>
-      <c r="E124" s="235"/>
-      <c r="F124" s="235"/>
-      <c r="G124" s="235"/>
-      <c r="H124" s="235"/>
-      <c r="I124" s="235"/>
-      <c r="J124" s="235"/>
-      <c r="K124" s="235"/>
-      <c r="L124" s="235"/>
-      <c r="M124" s="235"/>
+      <c r="D124" s="233"/>
+      <c r="E124" s="233"/>
+      <c r="F124" s="233"/>
+      <c r="G124" s="233"/>
+      <c r="H124" s="233"/>
+      <c r="I124" s="233"/>
+      <c r="J124" s="233"/>
+      <c r="K124" s="233"/>
+      <c r="L124" s="233"/>
+      <c r="M124" s="233"/>
       <c r="N124" s="8" t="s">
         <v>521</v>
       </c>
@@ -46254,67 +46254,67 @@
       </c>
     </row>
     <row r="125" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="238"/>
+      <c r="A125" s="236"/>
       <c r="B125" s="28" t="s">
         <v>268</v>
       </c>
       <c r="C125" s="10" t="s">
         <v>436</v>
       </c>
-      <c r="D125" s="235"/>
-      <c r="E125" s="235"/>
-      <c r="F125" s="235"/>
-      <c r="G125" s="235"/>
-      <c r="H125" s="235"/>
-      <c r="I125" s="235"/>
-      <c r="J125" s="235"/>
-      <c r="K125" s="235"/>
-      <c r="L125" s="235"/>
-      <c r="M125" s="235"/>
-      <c r="N125" s="235" t="s">
+      <c r="D125" s="233"/>
+      <c r="E125" s="233"/>
+      <c r="F125" s="233"/>
+      <c r="G125" s="233"/>
+      <c r="H125" s="233"/>
+      <c r="I125" s="233"/>
+      <c r="J125" s="233"/>
+      <c r="K125" s="233"/>
+      <c r="L125" s="233"/>
+      <c r="M125" s="233"/>
+      <c r="N125" s="233" t="s">
         <v>1422</v>
       </c>
-      <c r="O125" s="235"/>
+      <c r="O125" s="233"/>
     </row>
     <row r="126" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="238"/>
+      <c r="A126" s="236"/>
       <c r="B126" s="28" t="s">
         <v>275</v>
       </c>
       <c r="C126" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="D126" s="235"/>
-      <c r="E126" s="235"/>
-      <c r="F126" s="235"/>
-      <c r="G126" s="235"/>
-      <c r="H126" s="235"/>
-      <c r="I126" s="235"/>
-      <c r="J126" s="235"/>
-      <c r="K126" s="235"/>
-      <c r="L126" s="235"/>
-      <c r="M126" s="235"/>
-      <c r="N126" s="235"/>
-      <c r="O126" s="235"/>
+      <c r="D126" s="233"/>
+      <c r="E126" s="233"/>
+      <c r="F126" s="233"/>
+      <c r="G126" s="233"/>
+      <c r="H126" s="233"/>
+      <c r="I126" s="233"/>
+      <c r="J126" s="233"/>
+      <c r="K126" s="233"/>
+      <c r="L126" s="233"/>
+      <c r="M126" s="233"/>
+      <c r="N126" s="233"/>
+      <c r="O126" s="233"/>
     </row>
     <row r="127" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="238"/>
+      <c r="A127" s="236"/>
       <c r="B127" s="115" t="s">
         <v>86</v>
       </c>
       <c r="C127" s="10" t="s">
         <v>1291</v>
       </c>
-      <c r="D127" s="235"/>
-      <c r="E127" s="235"/>
-      <c r="F127" s="235"/>
-      <c r="G127" s="235"/>
-      <c r="H127" s="235"/>
-      <c r="I127" s="235"/>
-      <c r="J127" s="235"/>
-      <c r="K127" s="235"/>
-      <c r="L127" s="235"/>
-      <c r="M127" s="235"/>
+      <c r="D127" s="233"/>
+      <c r="E127" s="233"/>
+      <c r="F127" s="233"/>
+      <c r="G127" s="233"/>
+      <c r="H127" s="233"/>
+      <c r="I127" s="233"/>
+      <c r="J127" s="233"/>
+      <c r="K127" s="233"/>
+      <c r="L127" s="233"/>
+      <c r="M127" s="233"/>
       <c r="N127" s="8" t="s">
         <v>523</v>
       </c>
@@ -46324,7 +46324,7 @@
     </row>
     <row r="128" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="129" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="236" t="s">
+      <c r="A129" s="229" t="s">
         <v>299</v>
       </c>
       <c r="B129" s="24" t="s">
@@ -46333,78 +46333,78 @@
       <c r="C129" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="D129" s="235" t="s">
+      <c r="D129" s="233" t="s">
         <v>1423</v>
       </c>
-      <c r="E129" s="235"/>
-      <c r="F129" s="235"/>
-      <c r="G129" s="235"/>
-      <c r="H129" s="235"/>
-      <c r="I129" s="235"/>
-      <c r="J129" s="235"/>
-      <c r="K129" s="235"/>
-      <c r="L129" s="235"/>
-      <c r="M129" s="235"/>
-      <c r="N129" s="235"/>
-      <c r="O129" s="235"/>
-      <c r="P129" s="235"/>
-      <c r="Q129" s="235"/>
-      <c r="R129" s="235"/>
-      <c r="S129" s="235"/>
+      <c r="E129" s="233"/>
+      <c r="F129" s="233"/>
+      <c r="G129" s="233"/>
+      <c r="H129" s="233"/>
+      <c r="I129" s="233"/>
+      <c r="J129" s="233"/>
+      <c r="K129" s="233"/>
+      <c r="L129" s="233"/>
+      <c r="M129" s="233"/>
+      <c r="N129" s="233"/>
+      <c r="O129" s="233"/>
+      <c r="P129" s="233"/>
+      <c r="Q129" s="233"/>
+      <c r="R129" s="233"/>
+      <c r="S129" s="233"/>
     </row>
     <row r="130" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="236"/>
+      <c r="A130" s="229"/>
       <c r="B130" s="24" t="s">
         <v>300</v>
       </c>
       <c r="C130" s="24" t="s">
         <v>441</v>
       </c>
-      <c r="D130" s="235"/>
-      <c r="E130" s="235"/>
-      <c r="F130" s="235"/>
-      <c r="G130" s="235"/>
-      <c r="H130" s="235"/>
-      <c r="I130" s="235"/>
-      <c r="J130" s="235"/>
-      <c r="K130" s="235"/>
-      <c r="L130" s="235"/>
-      <c r="M130" s="235"/>
-      <c r="N130" s="235"/>
-      <c r="O130" s="235"/>
-      <c r="P130" s="235"/>
-      <c r="Q130" s="235"/>
-      <c r="R130" s="235"/>
-      <c r="S130" s="235"/>
+      <c r="D130" s="233"/>
+      <c r="E130" s="233"/>
+      <c r="F130" s="233"/>
+      <c r="G130" s="233"/>
+      <c r="H130" s="233"/>
+      <c r="I130" s="233"/>
+      <c r="J130" s="233"/>
+      <c r="K130" s="233"/>
+      <c r="L130" s="233"/>
+      <c r="M130" s="233"/>
+      <c r="N130" s="233"/>
+      <c r="O130" s="233"/>
+      <c r="P130" s="233"/>
+      <c r="Q130" s="233"/>
+      <c r="R130" s="233"/>
+      <c r="S130" s="233"/>
     </row>
     <row r="131" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="236"/>
+      <c r="A131" s="229"/>
       <c r="B131" s="24" t="s">
         <v>121</v>
       </c>
       <c r="C131" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="D131" s="235"/>
-      <c r="E131" s="235"/>
-      <c r="F131" s="235"/>
-      <c r="G131" s="235"/>
-      <c r="H131" s="235"/>
-      <c r="I131" s="235"/>
-      <c r="J131" s="235"/>
-      <c r="K131" s="235"/>
-      <c r="L131" s="235"/>
-      <c r="M131" s="235"/>
-      <c r="N131" s="235"/>
-      <c r="O131" s="235"/>
-      <c r="P131" s="235"/>
-      <c r="Q131" s="235"/>
-      <c r="R131" s="235"/>
-      <c r="S131" s="235"/>
+      <c r="D131" s="233"/>
+      <c r="E131" s="233"/>
+      <c r="F131" s="233"/>
+      <c r="G131" s="233"/>
+      <c r="H131" s="233"/>
+      <c r="I131" s="233"/>
+      <c r="J131" s="233"/>
+      <c r="K131" s="233"/>
+      <c r="L131" s="233"/>
+      <c r="M131" s="233"/>
+      <c r="N131" s="233"/>
+      <c r="O131" s="233"/>
+      <c r="P131" s="233"/>
+      <c r="Q131" s="233"/>
+      <c r="R131" s="233"/>
+      <c r="S131" s="233"/>
     </row>
     <row r="132" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="133" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A133" s="232" t="s">
+      <c r="A133" s="230" t="s">
         <v>301</v>
       </c>
       <c r="B133" s="6" t="s">
@@ -46447,7 +46447,7 @@
       </c>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A134" s="232"/>
+      <c r="A134" s="230"/>
       <c r="B134" s="6" t="s">
         <v>98</v>
       </c>
@@ -46494,7 +46494,7 @@
       <c r="Q134" s="10"/>
     </row>
     <row r="135" spans="1:19" s="7" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="232"/>
+      <c r="A135" s="230"/>
       <c r="B135" s="10" t="s">
         <v>267</v>
       </c>
@@ -46539,7 +46539,7 @@
       </c>
     </row>
     <row r="136" spans="1:19" s="181" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="232"/>
+      <c r="A136" s="230"/>
       <c r="B136" s="182" t="s">
         <v>1217</v>
       </c>
@@ -46568,7 +46568,7 @@
       </c>
     </row>
     <row r="137" spans="1:19" s="181" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="232"/>
+      <c r="A137" s="230"/>
       <c r="B137" s="182" t="s">
         <v>1234</v>
       </c>
@@ -46597,7 +46597,7 @@
       </c>
     </row>
     <row r="138" spans="1:19" s="181" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="232"/>
+      <c r="A138" s="230"/>
       <c r="B138" s="181" t="s">
         <v>1054</v>
       </c>
@@ -46634,7 +46634,7 @@
       </c>
     </row>
     <row r="139" spans="1:19" s="181" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="232"/>
+      <c r="A139" s="230"/>
       <c r="B139" s="182" t="s">
         <v>1432</v>
       </c>
@@ -46657,7 +46657,7 @@
       </c>
     </row>
     <row r="140" spans="1:19" s="181" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="232"/>
+      <c r="A140" s="230"/>
       <c r="B140" s="182" t="s">
         <v>1441</v>
       </c>
@@ -46698,7 +46698,7 @@
       </c>
     </row>
     <row r="141" spans="1:19" s="115" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="232"/>
+      <c r="A141" s="230"/>
       <c r="B141" s="10" t="s">
         <v>290</v>
       </c>
@@ -46729,7 +46729,7 @@
       </c>
     </row>
     <row r="142" spans="1:19" s="115" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="232"/>
+      <c r="A142" s="230"/>
       <c r="B142" s="10" t="s">
         <v>792</v>
       </c>
@@ -46760,7 +46760,7 @@
       </c>
     </row>
     <row r="143" spans="1:19" s="181" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="232"/>
+      <c r="A143" s="230"/>
       <c r="B143" s="181" t="s">
         <v>280</v>
       </c>
@@ -46775,7 +46775,7 @@
       </c>
     </row>
     <row r="144" spans="1:19" s="115" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="232"/>
+      <c r="A144" s="230"/>
       <c r="B144" s="10" t="s">
         <v>1353</v>
       </c>
@@ -46814,7 +46814,7 @@
       </c>
     </row>
     <row r="145" spans="1:19" s="115" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="232"/>
+      <c r="A145" s="230"/>
       <c r="B145" s="10" t="s">
         <v>476</v>
       </c>
@@ -46845,7 +46845,7 @@
       </c>
     </row>
     <row r="146" spans="1:19" s="115" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="232"/>
+      <c r="A146" s="230"/>
       <c r="B146" s="10" t="s">
         <v>86</v>
       </c>
@@ -46876,87 +46876,87 @@
       </c>
     </row>
     <row r="147" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A147" s="232"/>
+      <c r="A147" s="230"/>
       <c r="B147" s="24" t="s">
         <v>302</v>
       </c>
       <c r="C147" s="24" t="s">
         <v>299</v>
       </c>
-      <c r="D147" s="235" t="s">
+      <c r="D147" s="233" t="s">
         <v>1424</v>
       </c>
-      <c r="E147" s="235"/>
-      <c r="F147" s="235"/>
-      <c r="G147" s="235"/>
-      <c r="H147" s="235"/>
-      <c r="I147" s="235"/>
-      <c r="J147" s="235"/>
-      <c r="K147" s="235"/>
-      <c r="L147" s="235"/>
-      <c r="M147" s="235"/>
-      <c r="N147" s="235"/>
-      <c r="O147" s="235"/>
-      <c r="P147" s="235"/>
-      <c r="Q147" s="235"/>
-      <c r="R147" s="235"/>
-      <c r="S147" s="235"/>
+      <c r="E147" s="233"/>
+      <c r="F147" s="233"/>
+      <c r="G147" s="233"/>
+      <c r="H147" s="233"/>
+      <c r="I147" s="233"/>
+      <c r="J147" s="233"/>
+      <c r="K147" s="233"/>
+      <c r="L147" s="233"/>
+      <c r="M147" s="233"/>
+      <c r="N147" s="233"/>
+      <c r="O147" s="233"/>
+      <c r="P147" s="233"/>
+      <c r="Q147" s="233"/>
+      <c r="R147" s="233"/>
+      <c r="S147" s="233"/>
     </row>
     <row r="148" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A148" s="232"/>
+      <c r="A148" s="230"/>
       <c r="B148" s="24" t="s">
         <v>105</v>
       </c>
       <c r="C148" s="24" t="s">
         <v>322</v>
       </c>
-      <c r="D148" s="235"/>
-      <c r="E148" s="235"/>
-      <c r="F148" s="235"/>
-      <c r="G148" s="235"/>
-      <c r="H148" s="235"/>
-      <c r="I148" s="235"/>
-      <c r="J148" s="235"/>
-      <c r="K148" s="235"/>
-      <c r="L148" s="235"/>
-      <c r="M148" s="235"/>
-      <c r="N148" s="235"/>
-      <c r="O148" s="235"/>
-      <c r="P148" s="235"/>
-      <c r="Q148" s="235"/>
-      <c r="R148" s="235"/>
-      <c r="S148" s="235"/>
+      <c r="D148" s="233"/>
+      <c r="E148" s="233"/>
+      <c r="F148" s="233"/>
+      <c r="G148" s="233"/>
+      <c r="H148" s="233"/>
+      <c r="I148" s="233"/>
+      <c r="J148" s="233"/>
+      <c r="K148" s="233"/>
+      <c r="L148" s="233"/>
+      <c r="M148" s="233"/>
+      <c r="N148" s="233"/>
+      <c r="O148" s="233"/>
+      <c r="P148" s="233"/>
+      <c r="Q148" s="233"/>
+      <c r="R148" s="233"/>
+      <c r="S148" s="233"/>
     </row>
     <row r="149" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A149" s="232"/>
+      <c r="A149" s="230"/>
       <c r="B149" s="24" t="s">
         <v>27</v>
       </c>
       <c r="C149" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="D149" s="235"/>
-      <c r="E149" s="235"/>
-      <c r="F149" s="235"/>
-      <c r="G149" s="235"/>
-      <c r="H149" s="235"/>
-      <c r="I149" s="235"/>
-      <c r="J149" s="235"/>
-      <c r="K149" s="235"/>
-      <c r="L149" s="235"/>
-      <c r="M149" s="235"/>
-      <c r="N149" s="235"/>
-      <c r="O149" s="235"/>
-      <c r="P149" s="235"/>
-      <c r="Q149" s="235"/>
-      <c r="R149" s="235"/>
-      <c r="S149" s="235"/>
+      <c r="D149" s="233"/>
+      <c r="E149" s="233"/>
+      <c r="F149" s="233"/>
+      <c r="G149" s="233"/>
+      <c r="H149" s="233"/>
+      <c r="I149" s="233"/>
+      <c r="J149" s="233"/>
+      <c r="K149" s="233"/>
+      <c r="L149" s="233"/>
+      <c r="M149" s="233"/>
+      <c r="N149" s="233"/>
+      <c r="O149" s="233"/>
+      <c r="P149" s="233"/>
+      <c r="Q149" s="233"/>
+      <c r="R149" s="233"/>
+      <c r="S149" s="233"/>
     </row>
     <row r="150" spans="1:19" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C150" s="17"/>
     </row>
     <row r="151" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A151" s="232" t="s">
+      <c r="A151" s="230" t="s">
         <v>303</v>
       </c>
       <c r="B151" s="6" t="s">
@@ -46984,7 +46984,7 @@
       <c r="P151" s="10"/>
     </row>
     <row r="152" spans="1:19" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A152" s="232"/>
+      <c r="A152" s="230"/>
       <c r="B152" s="10" t="s">
         <v>2</v>
       </c>
@@ -47029,7 +47029,7 @@
       </c>
     </row>
     <row r="153" spans="1:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A153" s="232"/>
+      <c r="A153" s="230"/>
       <c r="B153" s="6" t="s">
         <v>304</v>
       </c>
@@ -47085,7 +47085,7 @@
       <c r="R154" s="17"/>
     </row>
     <row r="155" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A155" s="232" t="s">
+      <c r="A155" s="230" t="s">
         <v>305</v>
       </c>
       <c r="B155" s="6" t="s">
@@ -47132,7 +47132,7 @@
       </c>
     </row>
     <row r="156" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A156" s="232"/>
+      <c r="A156" s="230"/>
       <c r="B156" s="6" t="s">
         <v>98</v>
       </c>
@@ -47177,7 +47177,7 @@
       </c>
     </row>
     <row r="157" spans="1:19" ht="51" x14ac:dyDescent="0.2">
-      <c r="A157" s="232"/>
+      <c r="A157" s="230"/>
       <c r="B157" s="6" t="s">
         <v>267</v>
       </c>
@@ -47222,7 +47222,7 @@
       </c>
     </row>
     <row r="158" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A158" s="232"/>
+      <c r="A158" s="230"/>
       <c r="B158" s="6" t="s">
         <v>52</v>
       </c>
@@ -47267,7 +47267,7 @@
       </c>
     </row>
     <row r="159" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A159" s="232"/>
+      <c r="A159" s="230"/>
       <c r="B159" s="6" t="s">
         <v>31</v>
       </c>
@@ -47312,7 +47312,7 @@
       </c>
     </row>
     <row r="160" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A160" s="232"/>
+      <c r="A160" s="230"/>
       <c r="B160" s="6" t="s">
         <v>105</v>
       </c>
@@ -47335,7 +47335,7 @@
       </c>
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A161" s="232"/>
+      <c r="A161" s="230"/>
       <c r="B161" s="6" t="s">
         <v>22</v>
       </c>
@@ -47368,7 +47368,7 @@
       </c>
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A162" s="232"/>
+      <c r="A162" s="230"/>
       <c r="B162" s="6" t="s">
         <v>40</v>
       </c>
@@ -47413,7 +47413,7 @@
       </c>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A163" s="232"/>
+      <c r="A163" s="230"/>
       <c r="B163" s="6" t="s">
         <v>45</v>
       </c>
@@ -47458,7 +47458,7 @@
       </c>
     </row>
     <row r="164" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A164" s="232"/>
+      <c r="A164" s="230"/>
       <c r="B164" s="6" t="s">
         <v>46</v>
       </c>
@@ -47503,7 +47503,7 @@
       </c>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A165" s="232"/>
+      <c r="A165" s="230"/>
       <c r="B165" s="6" t="s">
         <v>306</v>
       </c>
@@ -47538,7 +47538,7 @@
       </c>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A166" s="232"/>
+      <c r="A166" s="230"/>
       <c r="B166" s="6" t="s">
         <v>307</v>
       </c>
@@ -47569,7 +47569,7 @@
       <c r="M166" s="8"/>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A167" s="232"/>
+      <c r="A167" s="230"/>
       <c r="B167" s="6" t="s">
         <v>137</v>
       </c>
@@ -47614,7 +47614,7 @@
       </c>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A168" s="232"/>
+      <c r="A168" s="230"/>
       <c r="B168" s="6" t="s">
         <v>135</v>
       </c>
@@ -47649,7 +47649,7 @@
       </c>
     </row>
     <row r="169" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A169" s="232"/>
+      <c r="A169" s="230"/>
       <c r="B169" s="6" t="s">
         <v>50</v>
       </c>
@@ -47694,7 +47694,7 @@
       </c>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A170" s="232"/>
+      <c r="A170" s="230"/>
       <c r="B170" s="6" t="s">
         <v>308</v>
       </c>
@@ -47719,7 +47719,7 @@
       <c r="O170" s="8"/>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A171" s="232"/>
+      <c r="A171" s="230"/>
       <c r="B171" s="10" t="s">
         <v>35</v>
       </c>
@@ -47764,7 +47764,7 @@
       </c>
     </row>
     <row r="172" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A172" s="232"/>
+      <c r="A172" s="230"/>
       <c r="B172" s="6" t="s">
         <v>309</v>
       </c>
@@ -47803,7 +47803,7 @@
       </c>
     </row>
     <row r="173" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A173" s="232"/>
+      <c r="A173" s="230"/>
       <c r="B173" s="6" t="s">
         <v>83</v>
       </c>
@@ -47848,7 +47848,7 @@
       </c>
     </row>
     <row r="174" spans="1:15" s="115" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A174" s="232"/>
+      <c r="A174" s="230"/>
       <c r="B174" s="115" t="s">
         <v>281</v>
       </c>
@@ -47893,7 +47893,7 @@
       </c>
     </row>
     <row r="175" spans="1:15" s="115" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A175" s="232"/>
+      <c r="A175" s="230"/>
       <c r="B175" s="12" t="s">
         <v>1425</v>
       </c>
@@ -47951,7 +47951,7 @@
       <c r="M176" s="17"/>
     </row>
     <row r="177" spans="1:19" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A177" s="233" t="s">
+      <c r="A177" s="237" t="s">
         <v>1435</v>
       </c>
       <c r="B177" s="11" t="s">
@@ -47994,7 +47994,7 @@
       <c r="S177" s="12"/>
     </row>
     <row r="178" spans="1:19" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A178" s="233"/>
+      <c r="A178" s="237"/>
       <c r="B178" s="11" t="s">
         <v>98</v>
       </c>
@@ -48039,7 +48039,7 @@
       <c r="S178" s="12"/>
     </row>
     <row r="179" spans="1:19" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A179" s="233"/>
+      <c r="A179" s="237"/>
       <c r="B179" s="11" t="s">
         <v>2</v>
       </c>
@@ -48093,7 +48093,7 @@
       <c r="M180" s="17"/>
     </row>
     <row r="181" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A181" s="232" t="s">
+      <c r="A181" s="230" t="s">
         <v>310</v>
       </c>
       <c r="B181" s="6" t="s">
@@ -48129,7 +48129,7 @@
       <c r="O181" s="10"/>
     </row>
     <row r="182" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A182" s="232"/>
+      <c r="A182" s="230"/>
       <c r="B182" s="6" t="s">
         <v>98</v>
       </c>
@@ -48174,7 +48174,7 @@
       </c>
     </row>
     <row r="183" spans="1:19" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A183" s="232"/>
+      <c r="A183" s="230"/>
       <c r="B183" s="6" t="s">
         <v>267</v>
       </c>
@@ -48201,7 +48201,7 @@
       </c>
     </row>
     <row r="184" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A184" s="232"/>
+      <c r="A184" s="230"/>
       <c r="B184" s="24" t="s">
         <v>311</v>
       </c>
@@ -48222,7 +48222,7 @@
       <c r="O184" s="24"/>
     </row>
     <row r="185" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A185" s="232"/>
+      <c r="A185" s="230"/>
       <c r="B185" s="24" t="s">
         <v>312</v>
       </c>
@@ -48246,7 +48246,7 @@
       <c r="C186" s="17"/>
     </row>
     <row r="187" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="232" t="s">
+      <c r="A187" s="230" t="s">
         <v>414</v>
       </c>
       <c r="B187" s="13" t="s">
@@ -48275,7 +48275,7 @@
       </c>
     </row>
     <row r="188" spans="1:19" s="13" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A188" s="232"/>
+      <c r="A188" s="230"/>
       <c r="B188" s="13" t="s">
         <v>98</v>
       </c>
@@ -48314,7 +48314,7 @@
       </c>
     </row>
     <row r="189" spans="1:19" s="13" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A189" s="232"/>
+      <c r="A189" s="230"/>
       <c r="B189" s="13" t="s">
         <v>40</v>
       </c>
@@ -48353,7 +48353,7 @@
       </c>
     </row>
     <row r="190" spans="1:19" s="13" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A190" s="232"/>
+      <c r="A190" s="230"/>
       <c r="B190" s="13" t="s">
         <v>415</v>
       </c>
@@ -48389,7 +48389,7 @@
       </c>
     </row>
     <row r="191" spans="1:19" s="13" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A191" s="232"/>
+      <c r="A191" s="230"/>
       <c r="B191" s="13" t="s">
         <v>416</v>
       </c>
@@ -48428,7 +48428,7 @@
       </c>
     </row>
     <row r="192" spans="1:19" s="115" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A192" s="232"/>
+      <c r="A192" s="230"/>
       <c r="B192" s="10" t="s">
         <v>2</v>
       </c>
@@ -48453,7 +48453,7 @@
       <c r="M192" s="12"/>
     </row>
     <row r="193" spans="1:15" s="115" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="232"/>
+      <c r="A193" s="230"/>
       <c r="B193" s="10" t="s">
         <v>27</v>
       </c>
@@ -48480,7 +48480,7 @@
       <c r="M194" s="22"/>
     </row>
     <row r="195" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A195" s="232" t="s">
+      <c r="A195" s="230" t="s">
         <v>313</v>
       </c>
       <c r="B195" s="6" t="s">
@@ -48517,7 +48517,7 @@
       <c r="O195" s="28"/>
     </row>
     <row r="196" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A196" s="232"/>
+      <c r="A196" s="230"/>
       <c r="B196" s="6" t="s">
         <v>98</v>
       </c>
@@ -48562,7 +48562,7 @@
       </c>
     </row>
     <row r="197" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A197" s="232"/>
+      <c r="A197" s="230"/>
       <c r="B197" s="6" t="s">
         <v>267</v>
       </c>
@@ -48595,7 +48595,7 @@
       </c>
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A198" s="232"/>
+      <c r="A198" s="230"/>
       <c r="B198" s="27" t="s">
         <v>1451</v>
       </c>
@@ -48620,7 +48620,7 @@
       <c r="C199" s="17"/>
     </row>
     <row r="200" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A200" s="232" t="s">
+      <c r="A200" s="230" t="s">
         <v>314</v>
       </c>
       <c r="B200" s="6" t="s">
@@ -48649,7 +48649,7 @@
       </c>
     </row>
     <row r="201" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A201" s="232"/>
+      <c r="A201" s="230"/>
       <c r="B201" s="6" t="s">
         <v>98</v>
       </c>
@@ -48688,7 +48688,7 @@
       </c>
     </row>
     <row r="202" spans="1:15" ht="51" x14ac:dyDescent="0.2">
-      <c r="A202" s="232"/>
+      <c r="A202" s="230"/>
       <c r="B202" s="6" t="s">
         <v>267</v>
       </c>
@@ -48715,7 +48715,7 @@
       </c>
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A203" s="232"/>
+      <c r="A203" s="230"/>
       <c r="B203" s="27" t="s">
         <v>315</v>
       </c>
@@ -48740,7 +48740,7 @@
       <c r="O203" s="24"/>
     </row>
     <row r="204" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A204" s="232"/>
+      <c r="A204" s="230"/>
       <c r="B204" s="27" t="s">
         <v>316</v>
       </c>
@@ -48777,7 +48777,7 @@
       <c r="C205" s="17"/>
     </row>
     <row r="206" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A206" s="232" t="s">
+      <c r="A206" s="230" t="s">
         <v>317</v>
       </c>
       <c r="B206" s="6" t="s">
@@ -48814,7 +48814,7 @@
       <c r="O206" s="28"/>
     </row>
     <row r="207" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A207" s="232"/>
+      <c r="A207" s="230"/>
       <c r="B207" s="6" t="s">
         <v>98</v>
       </c>
@@ -48859,7 +48859,7 @@
       </c>
     </row>
     <row r="208" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A208" s="232"/>
+      <c r="A208" s="230"/>
       <c r="B208" s="6" t="s">
         <v>267</v>
       </c>
@@ -48892,7 +48892,7 @@
       </c>
     </row>
     <row r="209" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A209" s="232"/>
+      <c r="A209" s="230"/>
       <c r="B209" s="24" t="s">
         <v>318</v>
       </c>
@@ -48921,13 +48921,13 @@
       <c r="C210" s="17"/>
     </row>
     <row r="211" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A211" s="237" t="s">
+      <c r="A211" s="231" t="s">
         <v>956</v>
       </c>
-      <c r="B211" s="234" t="s">
+      <c r="B211" s="235" t="s">
         <v>2</v>
       </c>
-      <c r="C211" s="234" t="s">
+      <c r="C211" s="235" t="s">
         <v>322</v>
       </c>
       <c r="D211" s="10" t="s">
@@ -48944,9 +48944,9 @@
       </c>
     </row>
     <row r="212" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A212" s="237"/>
-      <c r="B212" s="234"/>
-      <c r="C212" s="234"/>
+      <c r="A212" s="231"/>
+      <c r="B212" s="235"/>
+      <c r="C212" s="235"/>
       <c r="D212" s="10" t="s">
         <v>1221</v>
       </c>
@@ -48967,9 +48967,9 @@
       </c>
     </row>
     <row r="213" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A213" s="237"/>
-      <c r="B213" s="234"/>
-      <c r="C213" s="234"/>
+      <c r="A213" s="231"/>
+      <c r="B213" s="235"/>
+      <c r="C213" s="235"/>
       <c r="D213" s="10" t="s">
         <v>1222</v>
       </c>
@@ -48991,37 +48991,27 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A68:A76"/>
-    <mergeCell ref="A50:A55"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A10:A18"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A33:A44"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="D105:S105"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="D41:S42"/>
-    <mergeCell ref="D4:O8"/>
-    <mergeCell ref="D29:S31"/>
-    <mergeCell ref="D46:S48"/>
-    <mergeCell ref="D54:S54"/>
-    <mergeCell ref="D75:O75"/>
-    <mergeCell ref="D76:S76"/>
-    <mergeCell ref="D78:S81"/>
-    <mergeCell ref="D83:S86"/>
-    <mergeCell ref="D88:S97"/>
+    <mergeCell ref="M106:M107"/>
+    <mergeCell ref="N106:N107"/>
+    <mergeCell ref="O106:O107"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="E106:E107"/>
+    <mergeCell ref="H106:H107"/>
+    <mergeCell ref="I106:I107"/>
+    <mergeCell ref="J106:J107"/>
+    <mergeCell ref="K106:K107"/>
+    <mergeCell ref="F106:F107"/>
+    <mergeCell ref="G106:G107"/>
+    <mergeCell ref="L106:L107"/>
+    <mergeCell ref="A155:A175"/>
+    <mergeCell ref="A177:A179"/>
+    <mergeCell ref="C211:C213"/>
+    <mergeCell ref="N125:O126"/>
+    <mergeCell ref="N119:O119"/>
+    <mergeCell ref="N121:O122"/>
+    <mergeCell ref="D129:S131"/>
+    <mergeCell ref="D147:S149"/>
+    <mergeCell ref="D116:M127"/>
     <mergeCell ref="A78:A81"/>
     <mergeCell ref="A83:A86"/>
     <mergeCell ref="A88:A97"/>
@@ -49038,27 +49028,37 @@
     <mergeCell ref="A116:A127"/>
     <mergeCell ref="A187:A193"/>
     <mergeCell ref="A99:A109"/>
-    <mergeCell ref="A155:A175"/>
-    <mergeCell ref="A177:A179"/>
-    <mergeCell ref="C211:C213"/>
-    <mergeCell ref="N125:O126"/>
-    <mergeCell ref="N119:O119"/>
-    <mergeCell ref="N121:O122"/>
-    <mergeCell ref="D129:S131"/>
-    <mergeCell ref="D147:S149"/>
-    <mergeCell ref="D116:M127"/>
-    <mergeCell ref="M106:M107"/>
-    <mergeCell ref="N106:N107"/>
-    <mergeCell ref="O106:O107"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="E106:E107"/>
-    <mergeCell ref="H106:H107"/>
-    <mergeCell ref="I106:I107"/>
-    <mergeCell ref="J106:J107"/>
-    <mergeCell ref="K106:K107"/>
-    <mergeCell ref="F106:F107"/>
-    <mergeCell ref="G106:G107"/>
-    <mergeCell ref="L106:L107"/>
+    <mergeCell ref="D105:S105"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="D41:S42"/>
+    <mergeCell ref="D4:O8"/>
+    <mergeCell ref="D29:S31"/>
+    <mergeCell ref="D46:S48"/>
+    <mergeCell ref="D54:S54"/>
+    <mergeCell ref="D75:O75"/>
+    <mergeCell ref="D76:S76"/>
+    <mergeCell ref="D78:S81"/>
+    <mergeCell ref="D83:S86"/>
+    <mergeCell ref="D88:S97"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A10:A18"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A33:A44"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A68:A76"/>
+    <mergeCell ref="A50:A55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -49069,9 +49069,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>